<commit_message>
lag , named cells :  datum,domare,firstvaulter
</commit_message>
<xml_diff>
--- a/mallar/Protokoll_2017_lag_sv-r_mellan_justeras 2017-05-30.xlsx
+++ b/mallar/Protokoll_2017_lag_sv-r_mellan_justeras 2017-05-30.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21240" windowHeight="7140" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21240" windowHeight="7140" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="27" r:id="rId1"/>
@@ -29,6 +29,27 @@
     <definedName name="bord" localSheetId="7">'Lag kür art'!$L$3</definedName>
     <definedName name="bord" localSheetId="5">'Lag kür tekn jr mellan'!$L$3</definedName>
     <definedName name="bord" localSheetId="6">'Lag kür tekn sr'!$L$3</definedName>
+    <definedName name="datum" localSheetId="1">'Häst, lag'!$C$4</definedName>
+    <definedName name="datum" localSheetId="2">'Lag grund 1'!$C$4</definedName>
+    <definedName name="datum" localSheetId="3">'Lag grund 2'!$C$4</definedName>
+    <definedName name="datum" localSheetId="4">'Lag grund 3'!$C$4</definedName>
+    <definedName name="datum" localSheetId="7">'Lag kür art'!$C$4</definedName>
+    <definedName name="datum" localSheetId="5">'Lag kür tekn jr mellan'!$C$4</definedName>
+    <definedName name="datum" localSheetId="6">'Lag kür tekn sr'!$C$4</definedName>
+    <definedName name="domare" localSheetId="1">'Häst, lag'!$C$31</definedName>
+    <definedName name="domare" localSheetId="2">'Lag grund 1'!$C$33</definedName>
+    <definedName name="domare" localSheetId="3">'Lag grund 2'!$C$32</definedName>
+    <definedName name="domare" localSheetId="4">'Lag grund 3'!$C$33</definedName>
+    <definedName name="domare" localSheetId="7">'Lag kür art'!$C$27</definedName>
+    <definedName name="domare" localSheetId="5">'Lag kür tekn jr mellan'!$C$42</definedName>
+    <definedName name="domare" localSheetId="6">'Lag kür tekn sr'!$C$42</definedName>
+    <definedName name="firstvaulter" localSheetId="1">'Häst, lag'!$H$7</definedName>
+    <definedName name="firstvaulter" localSheetId="2">'Lag grund 1'!$I$7</definedName>
+    <definedName name="firstvaulter" localSheetId="3">'Lag grund 2'!$I$7</definedName>
+    <definedName name="firstvaulter" localSheetId="4">'Lag grund 3'!$I$7</definedName>
+    <definedName name="firstvaulter" localSheetId="7">'Lag kür art'!$I$7</definedName>
+    <definedName name="firstvaulter" localSheetId="5">'Lag kür tekn jr mellan'!$I$7</definedName>
+    <definedName name="firstvaulter" localSheetId="6">'Lag kür tekn sr'!$I$7</definedName>
     <definedName name="id" localSheetId="1">'Häst, lag'!$U$1</definedName>
     <definedName name="id" localSheetId="2">'Lag grund 1'!$U$1</definedName>
     <definedName name="id" localSheetId="3">'Lag grund 2'!$U$1</definedName>
@@ -2029,11 +2050,103 @@
     <xf numFmtId="167" fontId="2" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="51" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2043,23 +2156,12 @@
     <xf numFmtId="167" fontId="7" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
     <xf numFmtId="170" fontId="3" fillId="3" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2075,93 +2177,18 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="51" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -2176,12 +2203,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3416,8 +3437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A21" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27:K27"/>
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3483,9 +3504,9 @@
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="179"/>
-      <c r="D5" s="179"/>
-      <c r="E5" s="179"/>
+      <c r="C5" s="205"/>
+      <c r="D5" s="205"/>
+      <c r="E5" s="205"/>
       <c r="G5" s="11"/>
       <c r="H5" s="15" t="s">
         <v>17</v>
@@ -3499,9 +3520,9 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="179"/>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
+      <c r="C6" s="205"/>
+      <c r="D6" s="205"/>
+      <c r="E6" s="205"/>
       <c r="G6" s="1" t="s">
         <v>22</v>
       </c>
@@ -3517,77 +3538,77 @@
       <c r="G7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="180"/>
-      <c r="I7" s="181"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="182"/>
+      <c r="H7" s="204"/>
+      <c r="I7" s="213"/>
+      <c r="J7" s="213"/>
+      <c r="K7" s="214"/>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="180"/>
-      <c r="D8" s="180"/>
-      <c r="E8" s="180"/>
+      <c r="C8" s="204"/>
+      <c r="D8" s="204"/>
+      <c r="E8" s="204"/>
       <c r="G8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="179"/>
-      <c r="I8" s="185"/>
-      <c r="J8" s="185"/>
-      <c r="K8" s="186"/>
+      <c r="H8" s="205"/>
+      <c r="I8" s="206"/>
+      <c r="J8" s="206"/>
+      <c r="K8" s="207"/>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="205"/>
       <c r="G9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="179"/>
-      <c r="I9" s="185"/>
-      <c r="J9" s="185"/>
-      <c r="K9" s="186"/>
+      <c r="H9" s="205"/>
+      <c r="I9" s="206"/>
+      <c r="J9" s="206"/>
+      <c r="K9" s="207"/>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="179"/>
-      <c r="D10" s="179"/>
-      <c r="E10" s="179"/>
+      <c r="C10" s="205"/>
+      <c r="D10" s="205"/>
+      <c r="E10" s="205"/>
       <c r="G10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="179"/>
-      <c r="I10" s="185"/>
-      <c r="J10" s="185"/>
-      <c r="K10" s="186"/>
+      <c r="H10" s="205"/>
+      <c r="I10" s="206"/>
+      <c r="J10" s="206"/>
+      <c r="K10" s="207"/>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="179"/>
-      <c r="I11" s="185"/>
-      <c r="J11" s="185"/>
-      <c r="K11" s="186"/>
+      <c r="H11" s="205"/>
+      <c r="I11" s="206"/>
+      <c r="J11" s="206"/>
+      <c r="K11" s="207"/>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="18"/>
       <c r="G12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="179"/>
-      <c r="I12" s="185"/>
-      <c r="J12" s="185"/>
-      <c r="K12" s="186"/>
+      <c r="H12" s="205"/>
+      <c r="I12" s="206"/>
+      <c r="J12" s="206"/>
+      <c r="K12" s="207"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="18"/>
@@ -3598,44 +3619,44 @@
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G14" s="197" t="s">
+      <c r="G14" s="208" t="s">
         <v>61</v>
       </c>
-      <c r="H14" s="198"/>
-      <c r="I14" s="199" t="s">
+      <c r="H14" s="209"/>
+      <c r="I14" s="210" t="s">
         <v>101</v>
       </c>
-      <c r="J14" s="200"/>
-      <c r="K14" s="201"/>
+      <c r="J14" s="211"/>
+      <c r="K14" s="212"/>
     </row>
     <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="202" t="s">
+      <c r="A15" s="181" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="205" t="s">
+      <c r="B15" s="195" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="205" t="s">
+      <c r="C15" s="195" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="205"/>
-      <c r="E15" s="206" t="s">
+      <c r="D15" s="195"/>
+      <c r="E15" s="198" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="207"/>
+      <c r="F15" s="199"/>
       <c r="G15" s="51"/>
       <c r="H15" s="52"/>
-      <c r="I15" s="208" t="s">
+      <c r="I15" s="187" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="192"/>
-      <c r="K15" s="187">
+      <c r="J15" s="219"/>
+      <c r="K15" s="217">
         <f>ROUND(J15*0.3,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="203"/>
+      <c r="A16" s="182"/>
       <c r="B16" s="189"/>
       <c r="C16" s="189" t="s">
         <v>27</v>
@@ -3647,12 +3668,12 @@
       <c r="F16" s="191"/>
       <c r="G16" s="53"/>
       <c r="H16" s="54"/>
-      <c r="I16" s="209"/>
-      <c r="J16" s="193"/>
-      <c r="K16" s="188"/>
+      <c r="I16" s="188"/>
+      <c r="J16" s="220"/>
+      <c r="K16" s="218"/>
     </row>
     <row r="17" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="203"/>
+      <c r="A17" s="182"/>
       <c r="B17" s="189"/>
       <c r="C17" s="189" t="s">
         <v>26</v>
@@ -3664,13 +3685,13 @@
       <c r="F17" s="191"/>
       <c r="G17" s="55"/>
       <c r="H17" s="56"/>
-      <c r="I17" s="209"/>
-      <c r="J17" s="193"/>
-      <c r="K17" s="188"/>
+      <c r="I17" s="188"/>
+      <c r="J17" s="220"/>
+      <c r="K17" s="218"/>
     </row>
     <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="203"/>
-      <c r="B18" s="210" t="s">
+      <c r="A18" s="182"/>
+      <c r="B18" s="200" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="189" t="s">
@@ -3683,18 +3704,18 @@
       <c r="F18" s="191"/>
       <c r="G18" s="57"/>
       <c r="H18" s="58"/>
-      <c r="I18" s="209" t="s">
+      <c r="I18" s="188" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="193"/>
-      <c r="K18" s="188">
+      <c r="J18" s="220"/>
+      <c r="K18" s="218">
         <f>ROUND(J18*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="203"/>
-      <c r="B19" s="211"/>
+      <c r="A19" s="182"/>
+      <c r="B19" s="201"/>
       <c r="C19" s="189" t="s">
         <v>28</v>
       </c>
@@ -3705,56 +3726,56 @@
       <c r="F19" s="191"/>
       <c r="G19" s="53"/>
       <c r="H19" s="54"/>
-      <c r="I19" s="209"/>
-      <c r="J19" s="193"/>
-      <c r="K19" s="188"/>
+      <c r="I19" s="188"/>
+      <c r="J19" s="220"/>
+      <c r="K19" s="218"/>
     </row>
     <row r="20" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="204"/>
-      <c r="B20" s="212"/>
-      <c r="C20" s="214" t="s">
+      <c r="A20" s="183"/>
+      <c r="B20" s="202"/>
+      <c r="C20" s="192" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="214"/>
-      <c r="E20" s="215" t="s">
+      <c r="D20" s="192"/>
+      <c r="E20" s="193" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="216"/>
+      <c r="F20" s="194"/>
       <c r="G20" s="59"/>
       <c r="H20" s="60"/>
-      <c r="I20" s="213"/>
-      <c r="J20" s="194"/>
-      <c r="K20" s="195"/>
+      <c r="I20" s="203"/>
+      <c r="J20" s="221"/>
+      <c r="K20" s="222"/>
     </row>
     <row r="21" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="202" t="s">
+      <c r="A21" s="181" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="219" t="s">
+      <c r="B21" s="184" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="205" t="s">
+      <c r="C21" s="195" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="205"/>
-      <c r="E21" s="222" t="s">
+      <c r="D21" s="195"/>
+      <c r="E21" s="196" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="223"/>
+      <c r="F21" s="197"/>
       <c r="G21" s="61"/>
       <c r="H21" s="62"/>
-      <c r="I21" s="208" t="s">
+      <c r="I21" s="187" t="s">
         <v>105</v>
       </c>
-      <c r="J21" s="192"/>
-      <c r="K21" s="187">
+      <c r="J21" s="219"/>
+      <c r="K21" s="217">
         <f>ROUND(J21*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="203"/>
-      <c r="B22" s="220"/>
+      <c r="A22" s="182"/>
+      <c r="B22" s="185"/>
       <c r="C22" s="189" t="s">
         <v>31</v>
       </c>
@@ -3765,13 +3786,13 @@
       <c r="F22" s="191"/>
       <c r="G22" s="53"/>
       <c r="H22" s="54"/>
-      <c r="I22" s="209"/>
-      <c r="J22" s="193"/>
-      <c r="K22" s="188"/>
+      <c r="I22" s="188"/>
+      <c r="J22" s="220"/>
+      <c r="K22" s="218"/>
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="203"/>
-      <c r="B23" s="221"/>
+      <c r="A23" s="182"/>
+      <c r="B23" s="186"/>
       <c r="C23" s="189" t="s">
         <v>32</v>
       </c>
@@ -3782,21 +3803,21 @@
       <c r="F23" s="191"/>
       <c r="G23" s="55"/>
       <c r="H23" s="56"/>
-      <c r="I23" s="209"/>
-      <c r="J23" s="193"/>
-      <c r="K23" s="188"/>
+      <c r="I23" s="188"/>
+      <c r="J23" s="220"/>
+      <c r="K23" s="218"/>
     </row>
     <row r="24" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="204"/>
+      <c r="A24" s="183"/>
       <c r="B24" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="214"/>
-      <c r="D24" s="214"/>
-      <c r="E24" s="215" t="s">
+      <c r="C24" s="192"/>
+      <c r="D24" s="192"/>
+      <c r="E24" s="193" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="216"/>
+      <c r="F24" s="194"/>
       <c r="G24" s="64"/>
       <c r="H24" s="65"/>
       <c r="I24" s="66" t="s">
@@ -3815,14 +3836,14 @@
       <c r="B25" s="147" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="196" t="s">
+      <c r="C25" s="223" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="196"/>
-      <c r="E25" s="217" t="s">
+      <c r="D25" s="223"/>
+      <c r="E25" s="179" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="218"/>
+      <c r="F25" s="180"/>
       <c r="G25" s="68"/>
       <c r="H25" s="69"/>
       <c r="I25" s="70" t="s">
@@ -3859,11 +3880,11 @@
         <v>16</v>
       </c>
       <c r="I27" s="74"/>
-      <c r="J27" s="183">
+      <c r="J27" s="215">
         <f>SUM(K15:K25)</f>
         <v>0</v>
       </c>
-      <c r="K27" s="184"/>
+      <c r="K27" s="216"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
@@ -3884,40 +3905,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="C6:E6"/>
@@ -3934,6 +3921,40 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="J21:J23"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3949,7 +3970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
@@ -4014,10 +4035,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="179"/>
-      <c r="D5" s="179"/>
-      <c r="E5" s="179"/>
-      <c r="F5" s="179"/>
+      <c r="C5" s="205"/>
+      <c r="D5" s="205"/>
+      <c r="E5" s="205"/>
+      <c r="F5" s="205"/>
       <c r="H5" s="11"/>
       <c r="I5" s="15" t="s">
         <v>17</v>
@@ -4031,10 +4052,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="179"/>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
-      <c r="F6" s="179"/>
+      <c r="C6" s="205"/>
+      <c r="D6" s="205"/>
+      <c r="E6" s="205"/>
+      <c r="F6" s="205"/>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
@@ -4051,80 +4072,80 @@
       <c r="H7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="180"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="181"/>
+      <c r="I7" s="204"/>
+      <c r="J7" s="213"/>
+      <c r="K7" s="213"/>
+      <c r="L7" s="213"/>
     </row>
     <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="180"/>
-      <c r="D8" s="180"/>
-      <c r="E8" s="180"/>
-      <c r="F8" s="180"/>
+      <c r="C8" s="204"/>
+      <c r="D8" s="204"/>
+      <c r="E8" s="204"/>
+      <c r="F8" s="204"/>
       <c r="H8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="179"/>
-      <c r="J8" s="185"/>
-      <c r="K8" s="185"/>
-      <c r="L8" s="185"/>
+      <c r="I8" s="205"/>
+      <c r="J8" s="206"/>
+      <c r="K8" s="206"/>
+      <c r="L8" s="206"/>
     </row>
     <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="205"/>
+      <c r="F9" s="205"/>
       <c r="H9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="179"/>
-      <c r="J9" s="185"/>
-      <c r="K9" s="185"/>
-      <c r="L9" s="185"/>
+      <c r="I9" s="205"/>
+      <c r="J9" s="206"/>
+      <c r="K9" s="206"/>
+      <c r="L9" s="206"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="179"/>
-      <c r="D10" s="179"/>
-      <c r="E10" s="179"/>
-      <c r="F10" s="179"/>
+      <c r="C10" s="205"/>
+      <c r="D10" s="205"/>
+      <c r="E10" s="205"/>
+      <c r="F10" s="205"/>
       <c r="H10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="179"/>
-      <c r="J10" s="185"/>
-      <c r="K10" s="185"/>
-      <c r="L10" s="185"/>
+      <c r="I10" s="205"/>
+      <c r="J10" s="206"/>
+      <c r="K10" s="206"/>
+      <c r="L10" s="206"/>
     </row>
     <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="179"/>
-      <c r="J11" s="185"/>
-      <c r="K11" s="185"/>
-      <c r="L11" s="185"/>
+      <c r="I11" s="205"/>
+      <c r="J11" s="206"/>
+      <c r="K11" s="206"/>
+      <c r="L11" s="206"/>
     </row>
     <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="18"/>
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="179"/>
-      <c r="J12" s="185"/>
-      <c r="K12" s="185"/>
-      <c r="L12" s="185"/>
+      <c r="I12" s="205"/>
+      <c r="J12" s="206"/>
+      <c r="K12" s="206"/>
+      <c r="L12" s="206"/>
     </row>
     <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H13" s="4"/>
@@ -4172,12 +4193,12 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="231"/>
-      <c r="B16" s="232" t="s">
+      <c r="A16" s="224"/>
+      <c r="B16" s="225" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="225"/>
-      <c r="D16" s="225"/>
+      <c r="C16" s="226"/>
+      <c r="D16" s="226"/>
       <c r="E16" s="23"/>
       <c r="F16" s="170"/>
       <c r="G16" s="170"/>
@@ -4191,12 +4212,12 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="231"/>
-      <c r="B17" s="224" t="s">
+      <c r="A17" s="224"/>
+      <c r="B17" s="227" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="225"/>
-      <c r="D17" s="225"/>
+      <c r="C17" s="226"/>
+      <c r="D17" s="226"/>
       <c r="E17" s="23"/>
       <c r="F17" s="170"/>
       <c r="G17" s="170"/>
@@ -4210,11 +4231,11 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="224" t="s">
+      <c r="B18" s="227" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="225"/>
-      <c r="D18" s="225"/>
+      <c r="C18" s="226"/>
+      <c r="D18" s="226"/>
       <c r="E18" s="23"/>
       <c r="F18" s="170"/>
       <c r="G18" s="170"/>
@@ -4228,11 +4249,11 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="229" t="s">
+      <c r="B19" s="231" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="225"/>
-      <c r="D19" s="225"/>
+      <c r="C19" s="226"/>
+      <c r="D19" s="226"/>
       <c r="E19" s="23"/>
       <c r="F19" s="170"/>
       <c r="G19" s="170"/>
@@ -4246,12 +4267,12 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="224" t="s">
+      <c r="B20" s="227" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="225"/>
-      <c r="D20" s="225"/>
-      <c r="E20" s="230"/>
+      <c r="C20" s="226"/>
+      <c r="D20" s="226"/>
+      <c r="E20" s="232"/>
       <c r="F20" s="170"/>
       <c r="G20" s="170"/>
       <c r="H20" s="170"/>
@@ -4264,11 +4285,11 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="224" t="s">
+      <c r="B21" s="227" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="225"/>
-      <c r="D21" s="225"/>
+      <c r="C21" s="226"/>
+      <c r="D21" s="226"/>
       <c r="E21" s="23"/>
       <c r="F21" s="170"/>
       <c r="G21" s="170"/>
@@ -4282,12 +4303,12 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="226" t="s">
+      <c r="B22" s="228" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="227"/>
-      <c r="D22" s="227"/>
-      <c r="E22" s="228"/>
+      <c r="C22" s="229"/>
+      <c r="D22" s="229"/>
+      <c r="E22" s="230"/>
       <c r="F22" s="170"/>
       <c r="G22" s="170"/>
       <c r="H22" s="170"/>
@@ -4463,6 +4484,13 @@
     <row r="66" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:E20"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="I8:L8"/>
@@ -4475,13 +4503,6 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4499,7 +4520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -4564,10 +4585,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="179"/>
-      <c r="D5" s="179"/>
-      <c r="E5" s="179"/>
-      <c r="F5" s="179"/>
+      <c r="C5" s="205"/>
+      <c r="D5" s="205"/>
+      <c r="E5" s="205"/>
+      <c r="F5" s="205"/>
       <c r="H5" s="11"/>
       <c r="I5" s="15" t="s">
         <v>17</v>
@@ -4581,10 +4602,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="179"/>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
-      <c r="F6" s="179"/>
+      <c r="C6" s="205"/>
+      <c r="D6" s="205"/>
+      <c r="E6" s="205"/>
+      <c r="F6" s="205"/>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
@@ -4601,80 +4622,80 @@
       <c r="H7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="180"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="182"/>
+      <c r="I7" s="204"/>
+      <c r="J7" s="213"/>
+      <c r="K7" s="213"/>
+      <c r="L7" s="214"/>
     </row>
     <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="180"/>
-      <c r="D8" s="180"/>
-      <c r="E8" s="180"/>
-      <c r="F8" s="180"/>
+      <c r="C8" s="204"/>
+      <c r="D8" s="204"/>
+      <c r="E8" s="204"/>
+      <c r="F8" s="204"/>
       <c r="H8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="179"/>
-      <c r="J8" s="185"/>
-      <c r="K8" s="185"/>
-      <c r="L8" s="186"/>
+      <c r="I8" s="205"/>
+      <c r="J8" s="206"/>
+      <c r="K8" s="206"/>
+      <c r="L8" s="207"/>
     </row>
     <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="205"/>
+      <c r="F9" s="205"/>
       <c r="H9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="179"/>
-      <c r="J9" s="185"/>
-      <c r="K9" s="185"/>
-      <c r="L9" s="186"/>
+      <c r="I9" s="205"/>
+      <c r="J9" s="206"/>
+      <c r="K9" s="206"/>
+      <c r="L9" s="207"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="179"/>
-      <c r="D10" s="179"/>
-      <c r="E10" s="179"/>
-      <c r="F10" s="179"/>
+      <c r="C10" s="205"/>
+      <c r="D10" s="205"/>
+      <c r="E10" s="205"/>
+      <c r="F10" s="205"/>
       <c r="H10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="179"/>
-      <c r="J10" s="185"/>
-      <c r="K10" s="185"/>
-      <c r="L10" s="186"/>
+      <c r="I10" s="205"/>
+      <c r="J10" s="206"/>
+      <c r="K10" s="206"/>
+      <c r="L10" s="207"/>
     </row>
     <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="179"/>
-      <c r="J11" s="185"/>
-      <c r="K11" s="185"/>
-      <c r="L11" s="186"/>
+      <c r="I11" s="205"/>
+      <c r="J11" s="206"/>
+      <c r="K11" s="206"/>
+      <c r="L11" s="207"/>
     </row>
     <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="18"/>
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="179"/>
-      <c r="J12" s="185"/>
-      <c r="K12" s="185"/>
-      <c r="L12" s="186"/>
+      <c r="I12" s="205"/>
+      <c r="J12" s="206"/>
+      <c r="K12" s="206"/>
+      <c r="L12" s="207"/>
     </row>
     <row r="13" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
@@ -4715,12 +4736,12 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="231"/>
-      <c r="B15" s="232" t="s">
+      <c r="A15" s="224"/>
+      <c r="B15" s="225" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="225"/>
-      <c r="D15" s="225"/>
+      <c r="C15" s="226"/>
+      <c r="D15" s="226"/>
       <c r="E15" s="23"/>
       <c r="F15" s="170"/>
       <c r="G15" s="170"/>
@@ -4734,12 +4755,12 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="231"/>
-      <c r="B16" s="224" t="s">
+      <c r="A16" s="224"/>
+      <c r="B16" s="227" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="225"/>
-      <c r="D16" s="225"/>
+      <c r="C16" s="226"/>
+      <c r="D16" s="226"/>
       <c r="E16" s="23"/>
       <c r="F16" s="170"/>
       <c r="G16" s="170"/>
@@ -4753,11 +4774,11 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="224" t="s">
+      <c r="B17" s="227" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="225"/>
-      <c r="D17" s="225"/>
+      <c r="C17" s="226"/>
+      <c r="D17" s="226"/>
       <c r="E17" s="23"/>
       <c r="F17" s="170"/>
       <c r="G17" s="170"/>
@@ -4771,11 +4792,11 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="229" t="s">
+      <c r="B18" s="231" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="225"/>
-      <c r="D18" s="225"/>
+      <c r="C18" s="226"/>
+      <c r="D18" s="226"/>
       <c r="E18" s="23"/>
       <c r="F18" s="170"/>
       <c r="G18" s="170"/>
@@ -4807,11 +4828,11 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="224" t="s">
+      <c r="B20" s="227" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="225"/>
-      <c r="D20" s="225"/>
+      <c r="C20" s="226"/>
+      <c r="D20" s="226"/>
       <c r="E20" s="23"/>
       <c r="F20" s="170"/>
       <c r="G20" s="170"/>
@@ -4843,7 +4864,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="226" t="s">
+      <c r="B22" s="228" t="s">
         <v>69</v>
       </c>
       <c r="C22" s="235"/>
@@ -5004,6 +5025,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="I7:L7"/>
     <mergeCell ref="C6:F6"/>
@@ -5016,13 +5044,6 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="7.874015748031496E-2"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5037,7 +5058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -5102,10 +5123,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="179"/>
-      <c r="D5" s="179"/>
-      <c r="E5" s="179"/>
-      <c r="F5" s="179"/>
+      <c r="C5" s="205"/>
+      <c r="D5" s="205"/>
+      <c r="E5" s="205"/>
+      <c r="F5" s="205"/>
       <c r="H5" s="11"/>
       <c r="I5" s="15" t="s">
         <v>17</v>
@@ -5119,10 +5140,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="179"/>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
-      <c r="F6" s="179"/>
+      <c r="C6" s="205"/>
+      <c r="D6" s="205"/>
+      <c r="E6" s="205"/>
+      <c r="F6" s="205"/>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
@@ -5139,79 +5160,79 @@
       <c r="H7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="180"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="182"/>
+      <c r="I7" s="204"/>
+      <c r="J7" s="213"/>
+      <c r="K7" s="213"/>
+      <c r="L7" s="214"/>
     </row>
     <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="180"/>
-      <c r="D8" s="180"/>
-      <c r="E8" s="180"/>
-      <c r="F8" s="180"/>
+      <c r="C8" s="204"/>
+      <c r="D8" s="204"/>
+      <c r="E8" s="204"/>
+      <c r="F8" s="204"/>
       <c r="H8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="179"/>
-      <c r="J8" s="185"/>
-      <c r="K8" s="185"/>
-      <c r="L8" s="186"/>
+      <c r="I8" s="205"/>
+      <c r="J8" s="206"/>
+      <c r="K8" s="206"/>
+      <c r="L8" s="207"/>
     </row>
     <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="205"/>
+      <c r="F9" s="205"/>
       <c r="H9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="179"/>
-      <c r="J9" s="185"/>
-      <c r="K9" s="185"/>
-      <c r="L9" s="186"/>
+      <c r="I9" s="205"/>
+      <c r="J9" s="206"/>
+      <c r="K9" s="206"/>
+      <c r="L9" s="207"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="179"/>
-      <c r="D10" s="179"/>
-      <c r="E10" s="179"/>
-      <c r="F10" s="179"/>
+      <c r="C10" s="205"/>
+      <c r="D10" s="205"/>
+      <c r="E10" s="205"/>
+      <c r="F10" s="205"/>
       <c r="H10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="179"/>
-      <c r="J10" s="185"/>
-      <c r="K10" s="185"/>
-      <c r="L10" s="186"/>
+      <c r="I10" s="205"/>
+      <c r="J10" s="206"/>
+      <c r="K10" s="206"/>
+      <c r="L10" s="207"/>
     </row>
     <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="179"/>
-      <c r="J11" s="185"/>
-      <c r="K11" s="185"/>
-      <c r="L11" s="186"/>
+      <c r="I11" s="205"/>
+      <c r="J11" s="206"/>
+      <c r="K11" s="206"/>
+      <c r="L11" s="207"/>
     </row>
     <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="179"/>
-      <c r="J12" s="185"/>
-      <c r="K12" s="185"/>
-      <c r="L12" s="186"/>
+      <c r="I12" s="205"/>
+      <c r="J12" s="206"/>
+      <c r="K12" s="206"/>
+      <c r="L12" s="207"/>
     </row>
     <row r="13" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
@@ -5252,12 +5273,12 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="231"/>
-      <c r="B15" s="232" t="s">
+      <c r="A15" s="224"/>
+      <c r="B15" s="225" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="225"/>
-      <c r="D15" s="225"/>
+      <c r="C15" s="226"/>
+      <c r="D15" s="226"/>
       <c r="E15" s="23"/>
       <c r="F15" s="170"/>
       <c r="G15" s="170"/>
@@ -5271,12 +5292,12 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="231"/>
-      <c r="B16" s="224" t="s">
+      <c r="A16" s="224"/>
+      <c r="B16" s="227" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="225"/>
-      <c r="D16" s="225"/>
+      <c r="C16" s="226"/>
+      <c r="D16" s="226"/>
       <c r="E16" s="23"/>
       <c r="F16" s="170"/>
       <c r="G16" s="170"/>
@@ -5290,11 +5311,11 @@
       </c>
     </row>
     <row r="17" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="224" t="s">
+      <c r="B17" s="227" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="225"/>
-      <c r="D17" s="225"/>
+      <c r="C17" s="226"/>
+      <c r="D17" s="226"/>
       <c r="E17" s="23"/>
       <c r="F17" s="170"/>
       <c r="G17" s="170"/>
@@ -5326,11 +5347,11 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="224" t="s">
+      <c r="B19" s="227" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="225"/>
-      <c r="D19" s="225"/>
+      <c r="C19" s="226"/>
+      <c r="D19" s="226"/>
       <c r="E19" s="25"/>
       <c r="F19" s="170"/>
       <c r="G19" s="170"/>
@@ -5380,12 +5401,12 @@
       </c>
     </row>
     <row r="22" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="226" t="s">
+      <c r="B22" s="228" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="227"/>
-      <c r="D22" s="227"/>
-      <c r="E22" s="228"/>
+      <c r="C22" s="229"/>
+      <c r="D22" s="229"/>
+      <c r="E22" s="230"/>
       <c r="F22" s="170"/>
       <c r="G22" s="170"/>
       <c r="H22" s="170"/>
@@ -5545,6 +5566,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B22:E22"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="C8:F8"/>
@@ -5558,11 +5584,6 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B22:E22"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5577,7 +5598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
@@ -5644,10 +5665,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="179"/>
-      <c r="D5" s="179"/>
-      <c r="E5" s="179"/>
-      <c r="F5" s="179"/>
+      <c r="C5" s="205"/>
+      <c r="D5" s="205"/>
+      <c r="E5" s="205"/>
+      <c r="F5" s="205"/>
       <c r="H5" s="11"/>
       <c r="I5" s="15" t="s">
         <v>17</v>
@@ -5661,10 +5682,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="179"/>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
-      <c r="F6" s="179"/>
+      <c r="C6" s="205"/>
+      <c r="D6" s="205"/>
+      <c r="E6" s="205"/>
+      <c r="F6" s="205"/>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
@@ -5681,79 +5702,79 @@
       <c r="H7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="180"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="182"/>
+      <c r="I7" s="204"/>
+      <c r="J7" s="213"/>
+      <c r="K7" s="213"/>
+      <c r="L7" s="214"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="180"/>
-      <c r="D8" s="180"/>
-      <c r="E8" s="180"/>
-      <c r="F8" s="180"/>
+      <c r="C8" s="204"/>
+      <c r="D8" s="204"/>
+      <c r="E8" s="204"/>
+      <c r="F8" s="204"/>
       <c r="H8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="179"/>
-      <c r="J8" s="185"/>
-      <c r="K8" s="185"/>
-      <c r="L8" s="186"/>
+      <c r="I8" s="205"/>
+      <c r="J8" s="206"/>
+      <c r="K8" s="206"/>
+      <c r="L8" s="207"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="205"/>
+      <c r="F9" s="205"/>
       <c r="H9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="179"/>
-      <c r="J9" s="185"/>
-      <c r="K9" s="185"/>
-      <c r="L9" s="186"/>
+      <c r="I9" s="205"/>
+      <c r="J9" s="206"/>
+      <c r="K9" s="206"/>
+      <c r="L9" s="207"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="179"/>
-      <c r="D10" s="179"/>
-      <c r="E10" s="179"/>
-      <c r="F10" s="179"/>
+      <c r="C10" s="205"/>
+      <c r="D10" s="205"/>
+      <c r="E10" s="205"/>
+      <c r="F10" s="205"/>
       <c r="H10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="179"/>
-      <c r="J10" s="185"/>
-      <c r="K10" s="185"/>
-      <c r="L10" s="186"/>
+      <c r="I10" s="205"/>
+      <c r="J10" s="206"/>
+      <c r="K10" s="206"/>
+      <c r="L10" s="207"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="179"/>
-      <c r="J11" s="185"/>
-      <c r="K11" s="185"/>
-      <c r="L11" s="186"/>
+      <c r="I11" s="205"/>
+      <c r="J11" s="206"/>
+      <c r="K11" s="206"/>
+      <c r="L11" s="207"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="179"/>
-      <c r="J12" s="185"/>
-      <c r="K12" s="185"/>
-      <c r="L12" s="186"/>
+      <c r="I12" s="205"/>
+      <c r="J12" s="206"/>
+      <c r="K12" s="206"/>
+      <c r="L12" s="207"/>
     </row>
     <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H13" s="4"/>
@@ -6116,7 +6137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
@@ -6183,10 +6204,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="179"/>
-      <c r="D5" s="179"/>
-      <c r="E5" s="179"/>
-      <c r="F5" s="179"/>
+      <c r="C5" s="205"/>
+      <c r="D5" s="205"/>
+      <c r="E5" s="205"/>
+      <c r="F5" s="205"/>
       <c r="H5" s="11"/>
       <c r="I5" s="15" t="s">
         <v>17</v>
@@ -6200,10 +6221,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="179"/>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
-      <c r="F6" s="179"/>
+      <c r="C6" s="205"/>
+      <c r="D6" s="205"/>
+      <c r="E6" s="205"/>
+      <c r="F6" s="205"/>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
@@ -6220,79 +6241,79 @@
       <c r="H7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="180"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="182"/>
+      <c r="I7" s="204"/>
+      <c r="J7" s="213"/>
+      <c r="K7" s="213"/>
+      <c r="L7" s="214"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="180"/>
-      <c r="D8" s="180"/>
-      <c r="E8" s="180"/>
-      <c r="F8" s="180"/>
+      <c r="C8" s="204"/>
+      <c r="D8" s="204"/>
+      <c r="E8" s="204"/>
+      <c r="F8" s="204"/>
       <c r="H8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="179"/>
-      <c r="J8" s="185"/>
-      <c r="K8" s="185"/>
-      <c r="L8" s="186"/>
+      <c r="I8" s="205"/>
+      <c r="J8" s="206"/>
+      <c r="K8" s="206"/>
+      <c r="L8" s="207"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="205"/>
+      <c r="F9" s="205"/>
       <c r="H9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="179"/>
-      <c r="J9" s="185"/>
-      <c r="K9" s="185"/>
-      <c r="L9" s="186"/>
+      <c r="I9" s="205"/>
+      <c r="J9" s="206"/>
+      <c r="K9" s="206"/>
+      <c r="L9" s="207"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="179"/>
-      <c r="D10" s="179"/>
-      <c r="E10" s="179"/>
-      <c r="F10" s="179"/>
+      <c r="C10" s="205"/>
+      <c r="D10" s="205"/>
+      <c r="E10" s="205"/>
+      <c r="F10" s="205"/>
       <c r="H10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="179"/>
-      <c r="J10" s="185"/>
-      <c r="K10" s="185"/>
-      <c r="L10" s="186"/>
+      <c r="I10" s="205"/>
+      <c r="J10" s="206"/>
+      <c r="K10" s="206"/>
+      <c r="L10" s="207"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="179"/>
-      <c r="J11" s="185"/>
-      <c r="K11" s="185"/>
-      <c r="L11" s="186"/>
+      <c r="I11" s="205"/>
+      <c r="J11" s="206"/>
+      <c r="K11" s="206"/>
+      <c r="L11" s="207"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="179"/>
-      <c r="J12" s="185"/>
-      <c r="K12" s="185"/>
-      <c r="L12" s="186"/>
+      <c r="I12" s="205"/>
+      <c r="J12" s="206"/>
+      <c r="K12" s="206"/>
+      <c r="L12" s="207"/>
     </row>
     <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H13" s="4"/>
@@ -6667,7 +6688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A19" zoomScale="110" zoomScaleNormal="120" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScale="110" zoomScaleNormal="120" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -6734,10 +6755,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="179"/>
-      <c r="D5" s="179"/>
-      <c r="E5" s="179"/>
-      <c r="F5" s="179"/>
+      <c r="C5" s="205"/>
+      <c r="D5" s="205"/>
+      <c r="E5" s="205"/>
+      <c r="F5" s="205"/>
       <c r="H5" s="11"/>
       <c r="I5" s="15" t="s">
         <v>17</v>
@@ -6751,10 +6772,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="179"/>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
-      <c r="F6" s="179"/>
+      <c r="C6" s="205"/>
+      <c r="D6" s="205"/>
+      <c r="E6" s="205"/>
+      <c r="F6" s="205"/>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
@@ -6771,80 +6792,80 @@
       <c r="H7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="180"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="182"/>
+      <c r="I7" s="204"/>
+      <c r="J7" s="213"/>
+      <c r="K7" s="213"/>
+      <c r="L7" s="214"/>
     </row>
     <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="180"/>
-      <c r="D8" s="180"/>
-      <c r="E8" s="180"/>
-      <c r="F8" s="180"/>
+      <c r="C8" s="204"/>
+      <c r="D8" s="204"/>
+      <c r="E8" s="204"/>
+      <c r="F8" s="204"/>
       <c r="H8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="179"/>
-      <c r="J8" s="185"/>
-      <c r="K8" s="185"/>
-      <c r="L8" s="186"/>
+      <c r="I8" s="205"/>
+      <c r="J8" s="206"/>
+      <c r="K8" s="206"/>
+      <c r="L8" s="207"/>
     </row>
     <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="205"/>
+      <c r="F9" s="205"/>
       <c r="H9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="179"/>
-      <c r="J9" s="185"/>
-      <c r="K9" s="185"/>
-      <c r="L9" s="186"/>
+      <c r="I9" s="205"/>
+      <c r="J9" s="206"/>
+      <c r="K9" s="206"/>
+      <c r="L9" s="207"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="179"/>
-      <c r="D10" s="179"/>
-      <c r="E10" s="179"/>
-      <c r="F10" s="179"/>
+      <c r="C10" s="205"/>
+      <c r="D10" s="205"/>
+      <c r="E10" s="205"/>
+      <c r="F10" s="205"/>
       <c r="H10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="179"/>
-      <c r="J10" s="185"/>
-      <c r="K10" s="185"/>
-      <c r="L10" s="186"/>
+      <c r="I10" s="205"/>
+      <c r="J10" s="206"/>
+      <c r="K10" s="206"/>
+      <c r="L10" s="207"/>
     </row>
     <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="179"/>
-      <c r="J11" s="185"/>
-      <c r="K11" s="185"/>
-      <c r="L11" s="186"/>
+      <c r="I11" s="205"/>
+      <c r="J11" s="206"/>
+      <c r="K11" s="206"/>
+      <c r="L11" s="207"/>
     </row>
     <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="18"/>
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="179"/>
-      <c r="J12" s="185"/>
-      <c r="K12" s="185"/>
-      <c r="L12" s="186"/>
+      <c r="I12" s="205"/>
+      <c r="J12" s="206"/>
+      <c r="K12" s="206"/>
+      <c r="L12" s="207"/>
     </row>
     <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="18"/>
@@ -7036,6 +7057,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="I7:L7"/>
@@ -7047,13 +7075,6 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7065,6 +7086,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7130,37 +7169,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7181,9 +7193,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ändrat rubriker på mallar
</commit_message>
<xml_diff>
--- a/mallar/Protokoll_2017_lag_sv-r_mellan_justeras 2017-05-30.xlsx
+++ b/mallar/Protokoll_2017_lag_sv-r_mellan_justeras 2017-05-30.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlu\Documents\Source\Repos\voltigeScore\mallar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus.sandberg\Documents\Visual Studio 2015\Projects\VoltigeClosedXML\mallar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21240" windowHeight="7140" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21240" windowHeight="7140" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="27" r:id="rId1"/>
@@ -79,12 +79,12 @@
     <definedName name="result" localSheetId="5">'Lag kür tekn jr mellan'!$L$34</definedName>
     <definedName name="result" localSheetId="6">'Lag kür tekn sr'!$L$35</definedName>
   </definedNames>
-  <calcPr calcId="171027" calcMode="manual"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="157">
   <si>
     <t>1)</t>
   </si>
@@ -615,15 +615,6 @@
   </si>
   <si>
     <t>Grund 1</t>
-  </si>
-  <si>
-    <t>Grund 2</t>
-  </si>
-  <si>
-    <t>Grund 3</t>
-  </si>
-  <si>
-    <t>Lag kür svårklass junior/mellanklass</t>
   </si>
   <si>
     <t xml:space="preserve">Svår klass seniorlag kür </t>
@@ -715,6 +706,12 @@
 • Urval av övningar och övergångar i harmoni med hästen.
 </t>
     </r>
+  </si>
+  <si>
+    <t>Grund</t>
+  </si>
+  <si>
+    <t>Lag kür svårklass junior</t>
   </si>
 </sst>
 </file>
@@ -2251,13 +2248,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Dezimal 2" xfId="2"/>
     <cellStyle name="Dezimal 2 2" xfId="4"/>
     <cellStyle name="Excel Built-in Normal" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="3"/>
+    <cellStyle name="Tusental" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2278,7 +2275,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2604,46 +2601,46 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="18" width="15.7109375" customWidth="1"/>
+    <col min="1" max="18" width="15.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="164" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="164" customFormat="1" ht="20.65" x14ac:dyDescent="0.6">
       <c r="A1" s="163" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="164" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="164" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="164" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="164" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="164" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="164" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="164" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:8" s="148" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="164" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:8" s="148" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
       <c r="A5" s="148" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="149" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="149"/>
     </row>
-    <row r="9" spans="1:8" s="150" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" s="150" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A9" s="150" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="151" t="s">
         <v>110</v>
       </c>
@@ -2652,7 +2649,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="150" t="s">
         <v>112</v>
       </c>
@@ -2673,7 +2670,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="149" t="s">
         <v>121</v>
       </c>
@@ -2697,7 +2694,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="149"/>
       <c r="B13" s="154"/>
       <c r="C13" s="154"/>
@@ -2707,7 +2704,7 @@
       <c r="G13" s="154"/>
       <c r="H13" s="154"/>
     </row>
-    <row r="14" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="149" t="s">
         <v>122</v>
       </c>
@@ -2731,7 +2728,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="149"/>
       <c r="B15" s="154"/>
       <c r="C15" s="154"/>
@@ -2741,7 +2738,7 @@
       <c r="G15" s="154"/>
       <c r="H15" s="154"/>
     </row>
-    <row r="16" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="149" t="s">
         <v>123</v>
       </c>
@@ -2765,7 +2762,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="149"/>
       <c r="B17" s="156"/>
       <c r="C17" s="156"/>
@@ -2775,12 +2772,12 @@
       <c r="G17" s="156"/>
       <c r="H17" s="156"/>
     </row>
-    <row r="19" spans="1:10" s="150" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" s="150" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A19" s="150" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="151" t="s">
         <v>110</v>
       </c>
@@ -2789,7 +2786,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="150" t="s">
         <v>112</v>
       </c>
@@ -2815,7 +2812,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="149" t="s">
         <v>121</v>
       </c>
@@ -2844,7 +2841,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="149"/>
       <c r="B23" s="154"/>
       <c r="C23" s="154"/>
@@ -2855,7 +2852,7 @@
       <c r="H23" s="154"/>
       <c r="I23" s="154"/>
     </row>
-    <row r="24" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="149" t="s">
         <v>122</v>
       </c>
@@ -2884,7 +2881,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="149"/>
       <c r="B25" s="154"/>
       <c r="C25" s="154"/>
@@ -2895,7 +2892,7 @@
       <c r="H25" s="154"/>
       <c r="I25" s="154"/>
     </row>
-    <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="149" t="s">
         <v>123</v>
       </c>
@@ -2924,30 +2921,30 @@
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B27" s="155"/>
       <c r="C27" s="155"/>
       <c r="D27" s="155"/>
       <c r="E27" s="155"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B28" s="155"/>
       <c r="C28" s="155"/>
       <c r="D28" s="155"/>
       <c r="E28" s="155"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B29" s="155"/>
       <c r="C29" s="155"/>
       <c r="D29" s="155"/>
       <c r="E29" s="155"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A30" s="150" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="151" t="s">
         <v>110</v>
       </c>
@@ -2959,7 +2956,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B33" s="150" t="s">
         <v>112</v>
       </c>
@@ -2989,7 +2986,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="149" t="s">
         <v>121</v>
       </c>
@@ -3022,7 +3019,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="149"/>
       <c r="B35" s="154"/>
       <c r="C35" s="154"/>
@@ -3035,7 +3032,7 @@
       <c r="K35" s="154"/>
       <c r="L35" s="154"/>
     </row>
-    <row r="36" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="149" t="s">
         <v>122</v>
       </c>
@@ -3068,7 +3065,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="149"/>
       <c r="B37" s="154"/>
       <c r="C37" s="154"/>
@@ -3081,7 +3078,7 @@
       <c r="K37" s="154"/>
       <c r="L37" s="154"/>
     </row>
-    <row r="38" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="149" t="s">
         <v>123</v>
       </c>
@@ -3114,7 +3111,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="149"/>
       <c r="B39" s="155"/>
       <c r="C39" s="155"/>
@@ -3127,7 +3124,7 @@
       <c r="K39" s="155"/>
       <c r="L39" s="155"/>
     </row>
-    <row r="40" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="149"/>
       <c r="B40" s="155"/>
       <c r="C40" s="155"/>
@@ -3140,12 +3137,12 @@
       <c r="K40" s="155"/>
       <c r="L40" s="155"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A42" s="150" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="151" t="s">
         <v>110</v>
       </c>
@@ -3159,7 +3156,7 @@
       <c r="K44" s="149"/>
       <c r="N44" s="151"/>
     </row>
-    <row r="45" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B45" s="150" t="s">
         <v>112</v>
       </c>
@@ -3201,7 +3198,7 @@
       <c r="P45" s="150"/>
       <c r="Q45" s="150"/>
     </row>
-    <row r="46" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="149" t="s">
         <v>121</v>
       </c>
@@ -3242,7 +3239,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="149"/>
       <c r="B47" s="154"/>
       <c r="C47" s="154"/>
@@ -3257,7 +3254,7 @@
       <c r="L47" s="154"/>
       <c r="M47" s="154"/>
     </row>
-    <row r="48" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="149" t="s">
         <v>122</v>
       </c>
@@ -3298,7 +3295,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="149"/>
       <c r="B49" s="154"/>
       <c r="C49" s="154"/>
@@ -3313,7 +3310,7 @@
       <c r="L49" s="154"/>
       <c r="M49" s="154"/>
     </row>
-    <row r="50" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="149" t="s">
         <v>123</v>
       </c>
@@ -3354,12 +3351,12 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:13" s="162" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" s="162" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
       <c r="A53" s="161" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="160" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" s="160" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A54" s="159"/>
       <c r="B54" s="159" t="s">
         <v>112</v>
@@ -3377,7 +3374,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="158" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" s="158" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="157" t="s">
         <v>134</v>
       </c>
@@ -3397,7 +3394,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="56" spans="1:13" s="158" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" s="158" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="157" t="s">
         <v>139</v>
       </c>
@@ -3417,7 +3414,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="158" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" s="158" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A57" s="157"/>
       <c r="B57" s="157"/>
       <c r="C57" s="157"/>
@@ -3441,25 +3438,25 @@
       <selection activeCell="H7" sqref="H7:K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="50" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="50" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="50" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="50" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="50" customWidth="1"/>
+    <col min="1" max="1" width="5.73046875" style="50" customWidth="1"/>
+    <col min="2" max="2" width="10.265625" style="50" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.73046875" style="50" customWidth="1"/>
+    <col min="5" max="5" width="7.265625" style="50" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" style="50" customWidth="1"/>
     <col min="7" max="7" width="7" style="50" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="50" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" style="50" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" style="50" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="50" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" style="50" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="50"/>
+    <col min="8" max="8" width="9.59765625" style="50" customWidth="1"/>
+    <col min="9" max="9" width="5.73046875" style="50" customWidth="1"/>
+    <col min="10" max="10" width="5.59765625" style="50" customWidth="1"/>
+    <col min="11" max="11" width="7.1328125" style="50" customWidth="1"/>
+    <col min="12" max="12" width="7.265625" style="50" customWidth="1"/>
+    <col min="13" max="16384" width="9.1328125" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
@@ -3471,7 +3468,7 @@
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -3483,7 +3480,7 @@
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -3499,7 +3496,7 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
@@ -3515,7 +3512,7 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -3527,7 +3524,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>102</v>
       </c>
@@ -3543,7 +3540,7 @@
       <c r="J7" s="213"/>
       <c r="K7" s="214"/>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -3559,7 +3556,7 @@
       <c r="J8" s="206"/>
       <c r="K8" s="207"/>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
@@ -3575,7 +3572,7 @@
       <c r="J9" s="206"/>
       <c r="K9" s="207"/>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
@@ -3591,7 +3588,7 @@
       <c r="J10" s="206"/>
       <c r="K10" s="207"/>
     </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="17" t="s">
         <v>4</v>
       </c>
@@ -3600,7 +3597,7 @@
       <c r="J11" s="206"/>
       <c r="K11" s="207"/>
     </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="18"/>
       <c r="G12" s="17" t="s">
         <v>5</v>
@@ -3610,7 +3607,7 @@
       <c r="J12" s="206"/>
       <c r="K12" s="207"/>
     </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="18"/>
       <c r="G13" s="4"/>
       <c r="H13" s="49"/>
@@ -3618,7 +3615,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G14" s="208" t="s">
         <v>61</v>
       </c>
@@ -3629,7 +3626,7 @@
       <c r="J14" s="211"/>
       <c r="K14" s="212"/>
     </row>
-    <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="181" t="s">
         <v>23</v>
       </c>
@@ -3655,7 +3652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="182"/>
       <c r="B16" s="189"/>
       <c r="C16" s="189" t="s">
@@ -3672,7 +3669,7 @@
       <c r="J16" s="220"/>
       <c r="K16" s="218"/>
     </row>
-    <row r="17" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="182"/>
       <c r="B17" s="189"/>
       <c r="C17" s="189" t="s">
@@ -3689,7 +3686,7 @@
       <c r="J17" s="220"/>
       <c r="K17" s="218"/>
     </row>
-    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="182"/>
       <c r="B18" s="200" t="s">
         <v>38</v>
@@ -3713,7 +3710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="182"/>
       <c r="B19" s="201"/>
       <c r="C19" s="189" t="s">
@@ -3730,7 +3727,7 @@
       <c r="J19" s="220"/>
       <c r="K19" s="218"/>
     </row>
-    <row r="20" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="183"/>
       <c r="B20" s="202"/>
       <c r="C20" s="192" t="s">
@@ -3747,7 +3744,7 @@
       <c r="J20" s="221"/>
       <c r="K20" s="222"/>
     </row>
-    <row r="21" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="181" t="s">
         <v>39</v>
       </c>
@@ -3773,7 +3770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="182"/>
       <c r="B22" s="185"/>
       <c r="C22" s="189" t="s">
@@ -3790,7 +3787,7 @@
       <c r="J22" s="220"/>
       <c r="K22" s="218"/>
     </row>
-    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="182"/>
       <c r="B23" s="186"/>
       <c r="C23" s="189" t="s">
@@ -3807,7 +3804,7 @@
       <c r="J23" s="220"/>
       <c r="K23" s="218"/>
     </row>
-    <row r="24" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="183"/>
       <c r="B24" s="63" t="s">
         <v>33</v>
@@ -3829,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="67" t="s">
         <v>40</v>
       </c>
@@ -3855,7 +3852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="72"/>
       <c r="B26" s="72"/>
       <c r="C26" s="72"/>
@@ -3868,7 +3865,7 @@
       <c r="J26" s="72"/>
       <c r="K26" s="72"/>
     </row>
-    <row r="27" spans="1:11" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="72"/>
       <c r="B27" s="72"/>
       <c r="C27" s="72"/>
@@ -3886,7 +3883,7 @@
       </c>
       <c r="K27" s="216"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>36</v>
       </c>
@@ -3974,22 +3971,22 @@
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="7.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="3" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.73046875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="7.265625" style="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" customWidth="1"/>
-    <col min="9" max="11" width="7.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="11" width="7.265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.59765625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>129</v>
       </c>
@@ -4001,7 +3998,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
     </row>
-    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>149</v>
       </c>
@@ -4013,7 +4010,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
     </row>
-    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -4030,7 +4027,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
@@ -4047,7 +4044,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -4060,7 +4057,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>102</v>
       </c>
@@ -4077,7 +4074,7 @@
       <c r="K7" s="213"/>
       <c r="L7" s="213"/>
     </row>
-    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -4094,7 +4091,7 @@
       <c r="K8" s="206"/>
       <c r="L8" s="206"/>
     </row>
-    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
@@ -4111,7 +4108,7 @@
       <c r="K9" s="206"/>
       <c r="L9" s="206"/>
     </row>
-    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
@@ -4128,7 +4125,7 @@
       <c r="K10" s="206"/>
       <c r="L10" s="206"/>
     </row>
-    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
@@ -4137,7 +4134,7 @@
       <c r="K11" s="206"/>
       <c r="L11" s="206"/>
     </row>
-    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="18"/>
       <c r="H12" s="17" t="s">
         <v>5</v>
@@ -4147,14 +4144,14 @@
       <c r="K12" s="206"/>
       <c r="L12" s="206"/>
     </row>
-    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21"/>
@@ -4169,7 +4166,7 @@
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
     </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F15" s="22">
         <v>1</v>
       </c>
@@ -4192,7 +4189,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="224"/>
       <c r="B16" s="225" t="s">
         <v>54</v>
@@ -4211,7 +4208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="224"/>
       <c r="B17" s="227" t="s">
         <v>55</v>
@@ -4230,7 +4227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="227" t="s">
         <v>56</v>
       </c>
@@ -4248,7 +4245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="231" t="s">
         <v>57</v>
       </c>
@@ -4266,7 +4263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="227" t="s">
         <v>59</v>
       </c>
@@ -4284,7 +4281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="227" t="s">
         <v>58</v>
       </c>
@@ -4302,7 +4299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="228" t="s">
         <v>60</v>
       </c>
@@ -4320,10 +4317,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L23" s="26"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="27" t="s">
         <v>61</v>
       </c>
@@ -4341,7 +4338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="31"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
@@ -4358,7 +4355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B26" s="31"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -4370,7 +4367,7 @@
       <c r="J26" s="36"/>
       <c r="L26" s="37"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B27" s="38"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -4384,8 +4381,8 @@
       </c>
       <c r="L27" s="36"/>
     </row>
-    <row r="28" spans="1:12" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H29" s="40"/>
       <c r="I29" s="41" t="s">
         <v>65</v>
@@ -4397,7 +4394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
@@ -4409,7 +4406,7 @@
       <c r="K30" s="30"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
@@ -4421,8 +4418,8 @@
       <c r="K31" s="30"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -4439,7 +4436,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
@@ -4451,7 +4448,7 @@
       <c r="K34" s="30"/>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="48"/>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
@@ -4466,22 +4463,22 @@
       <c r="L35" s="48"/>
       <c r="M35" s="48"/>
     </row>
-    <row r="36" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="B21:D21"/>
@@ -4520,26 +4517,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="7.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="3" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.73046875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="7.265625" style="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" customWidth="1"/>
-    <col min="9" max="11" width="7.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="11" width="7.265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.59765625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>130</v>
       </c>
@@ -4551,9 +4548,9 @@
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
     </row>
-    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="15" t="s">
@@ -4563,7 +4560,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
     </row>
-    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -4580,7 +4577,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
@@ -4597,7 +4594,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -4610,7 +4607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>102</v>
       </c>
@@ -4627,7 +4624,7 @@
       <c r="K7" s="213"/>
       <c r="L7" s="214"/>
     </row>
-    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -4644,7 +4641,7 @@
       <c r="K8" s="206"/>
       <c r="L8" s="207"/>
     </row>
-    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
@@ -4661,7 +4658,7 @@
       <c r="K9" s="206"/>
       <c r="L9" s="207"/>
     </row>
-    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
@@ -4678,7 +4675,7 @@
       <c r="K10" s="206"/>
       <c r="L10" s="207"/>
     </row>
-    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
@@ -4687,7 +4684,7 @@
       <c r="K11" s="206"/>
       <c r="L11" s="207"/>
     </row>
-    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="18"/>
       <c r="H12" s="17" t="s">
         <v>5</v>
@@ -4697,7 +4694,7 @@
       <c r="K12" s="206"/>
       <c r="L12" s="207"/>
     </row>
-    <row r="13" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="20"/>
       <c r="C13" s="21"/>
@@ -4712,7 +4709,7 @@
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
     </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F14" s="22">
         <v>1</v>
       </c>
@@ -4735,7 +4732,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="224"/>
       <c r="B15" s="225" t="s">
         <v>54</v>
@@ -4754,7 +4751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="224"/>
       <c r="B16" s="227" t="s">
         <v>55</v>
@@ -4773,7 +4770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="227" t="s">
         <v>56</v>
       </c>
@@ -4791,7 +4788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="231" t="s">
         <v>66</v>
       </c>
@@ -4809,7 +4806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="233" t="s">
         <v>67</v>
       </c>
@@ -4827,7 +4824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="227" t="s">
         <v>68</v>
       </c>
@@ -4845,7 +4842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="76" t="s">
         <v>57</v>
       </c>
@@ -4863,7 +4860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="228" t="s">
         <v>69</v>
       </c>
@@ -4881,8 +4878,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="27" t="s">
         <v>61</v>
       </c>
@@ -4900,7 +4897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="31"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
@@ -4917,7 +4914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B26" s="31"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -4930,7 +4927,7 @@
       <c r="K26" s="21"/>
       <c r="L26" s="37"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B27" s="38"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -4944,8 +4941,8 @@
       </c>
       <c r="L27" s="36"/>
     </row>
-    <row r="28" spans="1:12" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F29" s="45"/>
       <c r="H29" s="40"/>
       <c r="I29" s="79" t="s">
@@ -4958,7 +4955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
@@ -4970,7 +4967,7 @@
       <c r="K30" s="30"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
@@ -4982,7 +4979,7 @@
       <c r="K31" s="30"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -4999,7 +4996,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
@@ -5011,7 +5008,7 @@
       <c r="K33" s="30"/>
       <c r="L33" s="8"/>
     </row>
-    <row r="34" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
@@ -5058,26 +5055,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="7.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="3" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.73046875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="7.265625" style="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" customWidth="1"/>
-    <col min="9" max="11" width="7.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="11" width="7.265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.59765625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>131</v>
       </c>
@@ -5089,9 +5086,9 @@
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
     </row>
-    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="15" t="s">
@@ -5101,7 +5098,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
     </row>
-    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -5118,7 +5115,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
@@ -5135,7 +5132,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -5148,7 +5145,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>102</v>
       </c>
@@ -5165,7 +5162,7 @@
       <c r="K7" s="213"/>
       <c r="L7" s="214"/>
     </row>
-    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -5182,7 +5179,7 @@
       <c r="K8" s="206"/>
       <c r="L8" s="207"/>
     </row>
-    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
@@ -5199,7 +5196,7 @@
       <c r="K9" s="206"/>
       <c r="L9" s="207"/>
     </row>
-    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
@@ -5216,7 +5213,7 @@
       <c r="K10" s="206"/>
       <c r="L10" s="207"/>
     </row>
-    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
@@ -5225,7 +5222,7 @@
       <c r="K11" s="206"/>
       <c r="L11" s="207"/>
     </row>
-    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
@@ -5234,7 +5231,7 @@
       <c r="K12" s="206"/>
       <c r="L12" s="207"/>
     </row>
-    <row r="13" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="20"/>
       <c r="C13" s="21"/>
@@ -5249,7 +5246,7 @@
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
     </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F14" s="22">
         <v>1</v>
       </c>
@@ -5272,7 +5269,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="224"/>
       <c r="B15" s="225" t="s">
         <v>54</v>
@@ -5291,7 +5288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="224"/>
       <c r="B16" s="227" t="s">
         <v>56</v>
@@ -5310,7 +5307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="227" t="s">
         <v>66</v>
       </c>
@@ -5328,7 +5325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="233" t="s">
         <v>67</v>
       </c>
@@ -5346,7 +5343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="227" t="s">
         <v>68</v>
       </c>
@@ -5364,7 +5361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="76" t="s">
         <v>57</v>
       </c>
@@ -5382,7 +5379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="76" t="s">
         <v>74</v>
       </c>
@@ -5400,7 +5397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="228" t="s">
         <v>75</v>
       </c>
@@ -5418,8 +5415,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="27" t="s">
         <v>61</v>
       </c>
@@ -5437,7 +5434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="31"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
@@ -5454,7 +5451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="31"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -5467,7 +5464,7 @@
       <c r="K26" s="21"/>
       <c r="L26" s="37"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="38"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -5481,8 +5478,8 @@
       </c>
       <c r="L27" s="36"/>
     </row>
-    <row r="28" spans="2:12" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F29" s="45"/>
       <c r="H29" s="40"/>
       <c r="I29" s="79" t="s">
@@ -5495,7 +5492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
@@ -5507,7 +5504,7 @@
       <c r="K30" s="30"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
@@ -5519,8 +5516,8 @@
       <c r="K31" s="30"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -5537,7 +5534,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
@@ -5549,7 +5546,7 @@
       <c r="K34" s="30"/>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="48"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -5598,30 +5595,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="7.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="3" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.73046875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="7.265625" style="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="7.265625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4.73046875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.73046875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="15" t="s">
@@ -5631,7 +5628,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
     </row>
-    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>76</v>
       </c>
@@ -5643,7 +5640,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
     </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -5660,7 +5657,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
@@ -5677,7 +5674,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -5690,7 +5687,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>102</v>
       </c>
@@ -5707,7 +5704,7 @@
       <c r="K7" s="213"/>
       <c r="L7" s="214"/>
     </row>
-    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -5724,7 +5721,7 @@
       <c r="K8" s="206"/>
       <c r="L8" s="207"/>
     </row>
-    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
@@ -5741,7 +5738,7 @@
       <c r="K9" s="206"/>
       <c r="L9" s="207"/>
     </row>
-    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
@@ -5758,7 +5755,7 @@
       <c r="K10" s="206"/>
       <c r="L10" s="207"/>
     </row>
-    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
@@ -5767,7 +5764,7 @@
       <c r="K11" s="206"/>
       <c r="L11" s="207"/>
     </row>
-    <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
@@ -5776,14 +5773,14 @@
       <c r="K12" s="206"/>
       <c r="L12" s="207"/>
     </row>
-    <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="82" t="s">
         <v>53</v>
       </c>
@@ -5799,7 +5796,7 @@
       <c r="K14" s="83"/>
       <c r="L14" s="84"/>
     </row>
-    <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -5813,7 +5810,7 @@
       <c r="K15" s="33"/>
       <c r="L15" s="85"/>
     </row>
-    <row r="16" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="31"/>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -5827,7 +5824,7 @@
       <c r="K16" s="21"/>
       <c r="L16" s="32"/>
     </row>
-    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="143" t="s">
         <v>73</v>
       </c>
@@ -5843,7 +5840,7 @@
       <c r="K17" s="145"/>
       <c r="L17" s="146"/>
     </row>
-    <row r="18" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="86" t="s">
         <v>78</v>
       </c>
@@ -5859,7 +5856,7 @@
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -5876,7 +5873,7 @@
       </c>
       <c r="M19" s="21"/>
     </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="122" t="s">
         <v>85</v>
       </c>
@@ -5895,7 +5892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="122" t="s">
         <v>86</v>
       </c>
@@ -5914,7 +5911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="122" t="s">
         <v>87</v>
       </c>
@@ -5933,7 +5930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="76" t="s">
         <v>88</v>
       </c>
@@ -5950,7 +5947,7 @@
       <c r="J23" s="26"/>
       <c r="K23" s="26"/>
     </row>
-    <row r="24" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G24" s="105" t="s">
         <v>91</v>
       </c>
@@ -5965,12 +5962,12 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="89"/>
       <c r="C26" s="89"/>
       <c r="D26" s="89"/>
@@ -5982,7 +5979,7 @@
       <c r="J26" s="91"/>
       <c r="K26" s="92"/>
     </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="76" t="s">
         <v>81</v>
       </c>
@@ -6007,7 +6004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="89"/>
       <c r="C28" s="89"/>
       <c r="D28" s="89"/>
@@ -6019,7 +6016,7 @@
       <c r="J28" s="91"/>
       <c r="K28" s="92"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
@@ -6031,7 +6028,7 @@
       <c r="J29" s="99"/>
       <c r="K29" s="100"/>
     </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
@@ -6045,7 +6042,7 @@
       <c r="J30" s="103"/>
       <c r="K30" s="172"/>
     </row>
-    <row r="31" spans="1:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
@@ -6057,7 +6054,7 @@
       <c r="K31" s="104"/>
       <c r="L31" s="88"/>
     </row>
-    <row r="32" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G32" s="105" t="s">
         <v>82</v>
       </c>
@@ -6072,8 +6069,8 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I34" s="79" t="s">
         <v>83</v>
       </c>
@@ -6084,16 +6081,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L35" s="140"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L36" s="140"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L37" s="140"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>36</v>
       </c>
@@ -6141,26 +6138,26 @@
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="7.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="3" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.73046875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="7.265625" style="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="7.265625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4.73046875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.73046875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="15" t="s">
@@ -6170,7 +6167,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
     </row>
-    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>76</v>
       </c>
@@ -6182,7 +6179,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
     </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -6199,7 +6196,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
@@ -6216,7 +6213,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -6229,7 +6226,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>102</v>
       </c>
@@ -6246,7 +6243,7 @@
       <c r="K7" s="213"/>
       <c r="L7" s="214"/>
     </row>
-    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -6263,7 +6260,7 @@
       <c r="K8" s="206"/>
       <c r="L8" s="207"/>
     </row>
-    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
@@ -6280,7 +6277,7 @@
       <c r="K9" s="206"/>
       <c r="L9" s="207"/>
     </row>
-    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
@@ -6297,7 +6294,7 @@
       <c r="K10" s="206"/>
       <c r="L10" s="207"/>
     </row>
-    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
@@ -6306,7 +6303,7 @@
       <c r="K11" s="206"/>
       <c r="L11" s="207"/>
     </row>
-    <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
@@ -6315,14 +6312,14 @@
       <c r="K12" s="206"/>
       <c r="L12" s="207"/>
     </row>
-    <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="82" t="s">
         <v>53</v>
       </c>
@@ -6338,7 +6335,7 @@
       <c r="K14" s="83"/>
       <c r="L14" s="84"/>
     </row>
-    <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -6352,7 +6349,7 @@
       <c r="K15" s="33"/>
       <c r="L15" s="85"/>
     </row>
-    <row r="16" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="31"/>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -6366,7 +6363,7 @@
       <c r="K16" s="21"/>
       <c r="L16" s="32"/>
     </row>
-    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="143" t="s">
         <v>73</v>
       </c>
@@ -6382,7 +6379,7 @@
       <c r="K17" s="145"/>
       <c r="L17" s="146"/>
     </row>
-    <row r="18" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="86" t="s">
         <v>78</v>
       </c>
@@ -6398,7 +6395,7 @@
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -6415,7 +6412,7 @@
       </c>
       <c r="M19" s="21"/>
     </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="122" t="s">
         <v>85</v>
       </c>
@@ -6435,7 +6432,7 @@
       </c>
       <c r="L20" s="26"/>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="122" t="s">
         <v>86</v>
       </c>
@@ -6455,7 +6452,7 @@
       </c>
       <c r="L21" s="26"/>
     </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="122" t="s">
         <v>87</v>
       </c>
@@ -6475,7 +6472,7 @@
       </c>
       <c r="L22" s="26"/>
     </row>
-    <row r="23" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="76" t="s">
         <v>88</v>
       </c>
@@ -6493,7 +6490,7 @@
       <c r="K23" s="126"/>
       <c r="L23" s="26"/>
     </row>
-    <row r="24" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
@@ -6513,7 +6510,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
@@ -6526,12 +6523,12 @@
       <c r="K25" s="134"/>
       <c r="L25" s="108"/>
     </row>
-    <row r="26" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="89"/>
       <c r="C27" s="89"/>
       <c r="D27" s="89"/>
@@ -6543,7 +6540,7 @@
       <c r="J27" s="91"/>
       <c r="K27" s="92"/>
     </row>
-    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="76" t="s">
         <v>81</v>
       </c>
@@ -6568,7 +6565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="89"/>
       <c r="C29" s="89"/>
       <c r="D29" s="89"/>
@@ -6580,7 +6577,7 @@
       <c r="J29" s="91"/>
       <c r="K29" s="92"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
@@ -6592,7 +6589,7 @@
       <c r="J30" s="99"/>
       <c r="K30" s="100"/>
     </row>
-    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
@@ -6606,7 +6603,7 @@
       <c r="J31" s="103"/>
       <c r="K31" s="172"/>
     </row>
-    <row r="32" spans="1:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
       <c r="D32" s="21"/>
@@ -6618,7 +6615,7 @@
       <c r="K32" s="104"/>
       <c r="L32" s="88"/>
     </row>
-    <row r="33" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G33" s="105" t="s">
         <v>82</v>
       </c>
@@ -6633,8 +6630,8 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I35" s="79" t="s">
         <v>83</v>
       </c>
@@ -6645,7 +6642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>36</v>
       </c>
@@ -6688,28 +6685,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScale="110" zoomScaleNormal="120" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" zoomScale="110" zoomScaleNormal="120" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="7.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="3" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.73046875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="7.265625" style="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="7.265625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4.73046875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.73046875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>132</v>
       </c>
@@ -6721,7 +6718,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
     </row>
-    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>77</v>
       </c>
@@ -6733,7 +6730,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
     </row>
-    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -6750,7 +6747,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
@@ -6767,7 +6764,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -6780,7 +6777,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>102</v>
       </c>
@@ -6797,7 +6794,7 @@
       <c r="K7" s="213"/>
       <c r="L7" s="214"/>
     </row>
-    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -6814,7 +6811,7 @@
       <c r="K8" s="206"/>
       <c r="L8" s="207"/>
     </row>
-    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
@@ -6831,7 +6828,7 @@
       <c r="K9" s="206"/>
       <c r="L9" s="207"/>
     </row>
-    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>100</v>
       </c>
@@ -6848,7 +6845,7 @@
       <c r="K10" s="206"/>
       <c r="L10" s="207"/>
     </row>
-    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
@@ -6857,7 +6854,7 @@
       <c r="K11" s="206"/>
       <c r="L11" s="207"/>
     </row>
-    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="18"/>
       <c r="H12" s="17" t="s">
         <v>5</v>
@@ -6867,7 +6864,7 @@
       <c r="K12" s="206"/>
       <c r="L12" s="207"/>
     </row>
-    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="18"/>
       <c r="H13" s="4"/>
       <c r="I13" s="49"/>
@@ -6875,7 +6872,7 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:13" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -6884,12 +6881,12 @@
       </c>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="236" t="s">
         <v>94</v>
       </c>
       <c r="B15" s="239" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C15" s="240"/>
       <c r="D15" s="240"/>
@@ -6908,10 +6905,10 @@
       </c>
       <c r="M15" s="113"/>
     </row>
-    <row r="16" spans="1:13" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="237"/>
       <c r="B16" s="242" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C16" s="243"/>
       <c r="D16" s="243"/>
@@ -6930,12 +6927,12 @@
       </c>
       <c r="M16" s="113"/>
     </row>
-    <row r="17" spans="1:13" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="236" t="s">
         <v>95</v>
       </c>
       <c r="B17" s="244" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C17" s="245"/>
       <c r="D17" s="245"/>
@@ -6954,7 +6951,7 @@
       </c>
       <c r="M17" s="113"/>
     </row>
-    <row r="18" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="238"/>
       <c r="B18" s="246" t="s">
         <v>99</v>
@@ -6976,7 +6973,7 @@
       </c>
       <c r="M18" s="113"/>
     </row>
-    <row r="19" spans="1:13" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="237"/>
       <c r="B19" s="242" t="s">
         <v>98</v>
@@ -6998,7 +6995,7 @@
       </c>
       <c r="M19" s="113"/>
     </row>
-    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K20" s="1" t="s">
         <v>35</v>
       </c>
@@ -7007,10 +7004,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L21" s="104"/>
     </row>
-    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="76" t="s">
         <v>80</v>
       </c>
@@ -7025,10 +7022,10 @@
       <c r="K22" s="77"/>
       <c r="L22" s="178"/>
     </row>
-    <row r="23" spans="1:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L23" s="104"/>
     </row>
-    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I24" s="79" t="s">
         <v>97</v>
       </c>
@@ -7039,7 +7036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Changed to text celltype for  competition class
</commit_message>
<xml_diff>
--- a/mallar/Protokoll_2017_lag_sv-r_mellan_justeras 2017-05-30.xlsx
+++ b/mallar/Protokoll_2017_lag_sv-r_mellan_justeras 2017-05-30.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus.sandberg\Documents\Visual Studio 2015\Projects\VoltigeClosedXML\mallar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AFEA55-F57A-4DCE-A833-6B95BF8E850F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB564C15-E722-4912-925D-164656E2A15B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21240" windowHeight="7140" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
     <definedName name="result" localSheetId="5">'Lag kür tekn jr mellan'!$L$34</definedName>
     <definedName name="result" localSheetId="6">'Lag kür tekn sr'!$L$35</definedName>
   </definedNames>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1593,7 +1593,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="248">
+  <cellXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2047,103 +2047,11 @@
     <xf numFmtId="167" fontId="2" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="51" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2153,12 +2061,23 @@
     <xf numFmtId="167" fontId="7" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
     <xf numFmtId="170" fontId="3" fillId="3" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2174,33 +2093,114 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="51" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2245,6 +2245,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3501,9 +3504,9 @@
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="205"/>
-      <c r="D5" s="205"/>
-      <c r="E5" s="205"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="179"/>
+      <c r="E5" s="179"/>
       <c r="G5" s="11"/>
       <c r="H5" s="15" t="s">
         <v>17</v>
@@ -3517,9 +3520,9 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="205"/>
-      <c r="D6" s="205"/>
-      <c r="E6" s="205"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
       <c r="G6" s="1" t="s">
         <v>22</v>
       </c>
@@ -3535,77 +3538,77 @@
       <c r="G7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="204"/>
-      <c r="I7" s="213"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="214"/>
+      <c r="H7" s="180"/>
+      <c r="I7" s="181"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="182"/>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="204"/>
-      <c r="D8" s="204"/>
-      <c r="E8" s="204"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="180"/>
       <c r="G8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="205"/>
-      <c r="I8" s="206"/>
-      <c r="J8" s="206"/>
-      <c r="K8" s="207"/>
+      <c r="H8" s="179"/>
+      <c r="I8" s="185"/>
+      <c r="J8" s="185"/>
+      <c r="K8" s="186"/>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="205"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
       <c r="G9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="205"/>
-      <c r="I9" s="206"/>
-      <c r="J9" s="206"/>
-      <c r="K9" s="207"/>
+      <c r="H9" s="179"/>
+      <c r="I9" s="185"/>
+      <c r="J9" s="185"/>
+      <c r="K9" s="186"/>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="205"/>
-      <c r="D10" s="205"/>
-      <c r="E10" s="205"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="179"/>
       <c r="G10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="205"/>
-      <c r="I10" s="206"/>
-      <c r="J10" s="206"/>
-      <c r="K10" s="207"/>
+      <c r="H10" s="179"/>
+      <c r="I10" s="185"/>
+      <c r="J10" s="185"/>
+      <c r="K10" s="186"/>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="205"/>
-      <c r="I11" s="206"/>
-      <c r="J11" s="206"/>
-      <c r="K11" s="207"/>
+      <c r="H11" s="179"/>
+      <c r="I11" s="185"/>
+      <c r="J11" s="185"/>
+      <c r="K11" s="186"/>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="18"/>
       <c r="G12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="205"/>
-      <c r="I12" s="206"/>
-      <c r="J12" s="206"/>
-      <c r="K12" s="207"/>
+      <c r="H12" s="179"/>
+      <c r="I12" s="185"/>
+      <c r="J12" s="185"/>
+      <c r="K12" s="186"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="18"/>
@@ -3616,44 +3619,44 @@
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G14" s="208" t="s">
+      <c r="G14" s="197" t="s">
         <v>61</v>
       </c>
-      <c r="H14" s="209"/>
-      <c r="I14" s="210" t="s">
+      <c r="H14" s="198"/>
+      <c r="I14" s="199" t="s">
         <v>100</v>
       </c>
-      <c r="J14" s="211"/>
-      <c r="K14" s="212"/>
+      <c r="J14" s="200"/>
+      <c r="K14" s="201"/>
     </row>
     <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="181" t="s">
+      <c r="A15" s="202" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="195" t="s">
+      <c r="B15" s="205" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="195" t="s">
+      <c r="C15" s="205" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="195"/>
-      <c r="E15" s="198" t="s">
+      <c r="D15" s="205"/>
+      <c r="E15" s="206" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="199"/>
+      <c r="F15" s="207"/>
       <c r="G15" s="51"/>
       <c r="H15" s="52"/>
-      <c r="I15" s="187" t="s">
+      <c r="I15" s="208" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="219"/>
-      <c r="K15" s="217">
+      <c r="J15" s="192"/>
+      <c r="K15" s="187">
         <f>ROUND(J15*0.3,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="182"/>
+      <c r="A16" s="203"/>
       <c r="B16" s="189"/>
       <c r="C16" s="189" t="s">
         <v>27</v>
@@ -3665,12 +3668,12 @@
       <c r="F16" s="191"/>
       <c r="G16" s="53"/>
       <c r="H16" s="54"/>
-      <c r="I16" s="188"/>
-      <c r="J16" s="220"/>
-      <c r="K16" s="218"/>
+      <c r="I16" s="209"/>
+      <c r="J16" s="193"/>
+      <c r="K16" s="188"/>
     </row>
     <row r="17" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="182"/>
+      <c r="A17" s="203"/>
       <c r="B17" s="189"/>
       <c r="C17" s="189" t="s">
         <v>26</v>
@@ -3682,13 +3685,13 @@
       <c r="F17" s="191"/>
       <c r="G17" s="55"/>
       <c r="H17" s="56"/>
-      <c r="I17" s="188"/>
-      <c r="J17" s="220"/>
-      <c r="K17" s="218"/>
+      <c r="I17" s="209"/>
+      <c r="J17" s="193"/>
+      <c r="K17" s="188"/>
     </row>
     <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="182"/>
-      <c r="B18" s="200" t="s">
+      <c r="A18" s="203"/>
+      <c r="B18" s="210" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="189" t="s">
@@ -3701,18 +3704,18 @@
       <c r="F18" s="191"/>
       <c r="G18" s="57"/>
       <c r="H18" s="58"/>
-      <c r="I18" s="188" t="s">
+      <c r="I18" s="209" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="220"/>
-      <c r="K18" s="218">
+      <c r="J18" s="193"/>
+      <c r="K18" s="188">
         <f>ROUND(J18*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="182"/>
-      <c r="B19" s="201"/>
+      <c r="A19" s="203"/>
+      <c r="B19" s="211"/>
       <c r="C19" s="189" t="s">
         <v>28</v>
       </c>
@@ -3723,56 +3726,56 @@
       <c r="F19" s="191"/>
       <c r="G19" s="53"/>
       <c r="H19" s="54"/>
-      <c r="I19" s="188"/>
-      <c r="J19" s="220"/>
-      <c r="K19" s="218"/>
+      <c r="I19" s="209"/>
+      <c r="J19" s="193"/>
+      <c r="K19" s="188"/>
     </row>
     <row r="20" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="183"/>
-      <c r="B20" s="202"/>
-      <c r="C20" s="192" t="s">
+      <c r="A20" s="204"/>
+      <c r="B20" s="212"/>
+      <c r="C20" s="214" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="192"/>
-      <c r="E20" s="193" t="s">
+      <c r="D20" s="214"/>
+      <c r="E20" s="215" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="194"/>
+      <c r="F20" s="216"/>
       <c r="G20" s="59"/>
       <c r="H20" s="60"/>
-      <c r="I20" s="203"/>
-      <c r="J20" s="221"/>
-      <c r="K20" s="222"/>
+      <c r="I20" s="213"/>
+      <c r="J20" s="194"/>
+      <c r="K20" s="195"/>
     </row>
     <row r="21" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="181" t="s">
+      <c r="A21" s="202" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="184" t="s">
+      <c r="B21" s="219" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="195" t="s">
+      <c r="C21" s="205" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="195"/>
-      <c r="E21" s="196" t="s">
+      <c r="D21" s="205"/>
+      <c r="E21" s="222" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="197"/>
+      <c r="F21" s="223"/>
       <c r="G21" s="61"/>
       <c r="H21" s="62"/>
-      <c r="I21" s="187" t="s">
+      <c r="I21" s="208" t="s">
         <v>104</v>
       </c>
-      <c r="J21" s="219"/>
-      <c r="K21" s="217">
+      <c r="J21" s="192"/>
+      <c r="K21" s="187">
         <f>ROUND(J21*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="182"/>
-      <c r="B22" s="185"/>
+      <c r="A22" s="203"/>
+      <c r="B22" s="220"/>
       <c r="C22" s="189" t="s">
         <v>31</v>
       </c>
@@ -3783,13 +3786,13 @@
       <c r="F22" s="191"/>
       <c r="G22" s="53"/>
       <c r="H22" s="54"/>
-      <c r="I22" s="188"/>
-      <c r="J22" s="220"/>
-      <c r="K22" s="218"/>
+      <c r="I22" s="209"/>
+      <c r="J22" s="193"/>
+      <c r="K22" s="188"/>
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="182"/>
-      <c r="B23" s="186"/>
+      <c r="A23" s="203"/>
+      <c r="B23" s="221"/>
       <c r="C23" s="189" t="s">
         <v>32</v>
       </c>
@@ -3800,21 +3803,21 @@
       <c r="F23" s="191"/>
       <c r="G23" s="55"/>
       <c r="H23" s="56"/>
-      <c r="I23" s="188"/>
-      <c r="J23" s="220"/>
-      <c r="K23" s="218"/>
+      <c r="I23" s="209"/>
+      <c r="J23" s="193"/>
+      <c r="K23" s="188"/>
     </row>
     <row r="24" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="183"/>
+      <c r="A24" s="204"/>
       <c r="B24" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="192"/>
-      <c r="D24" s="192"/>
-      <c r="E24" s="193" t="s">
+      <c r="C24" s="214"/>
+      <c r="D24" s="214"/>
+      <c r="E24" s="215" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="194"/>
+      <c r="F24" s="216"/>
       <c r="G24" s="64"/>
       <c r="H24" s="65"/>
       <c r="I24" s="66" t="s">
@@ -3833,14 +3836,14 @@
       <c r="B25" s="147" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="223" t="s">
+      <c r="C25" s="196" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="223"/>
-      <c r="E25" s="179" t="s">
+      <c r="D25" s="196"/>
+      <c r="E25" s="217" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="180"/>
+      <c r="F25" s="218"/>
       <c r="G25" s="68"/>
       <c r="H25" s="69"/>
       <c r="I25" s="70" t="s">
@@ -3877,11 +3880,11 @@
         <v>16</v>
       </c>
       <c r="I27" s="74"/>
-      <c r="J27" s="215">
+      <c r="J27" s="183">
         <f>SUM(K15:K25)</f>
         <v>0</v>
       </c>
-      <c r="K27" s="216"/>
+      <c r="K27" s="184"/>
     </row>
     <row r="31" spans="1:11" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
@@ -3902,6 +3905,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="C6:E6"/>
@@ -3918,40 +3955,6 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="J21:J23"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3967,8 +3970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -4025,17 +4028,17 @@
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="L4" s="248"/>
     </row>
     <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="205"/>
-      <c r="D5" s="205"/>
-      <c r="E5" s="205"/>
-      <c r="F5" s="205"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="179"/>
+      <c r="E5" s="179"/>
+      <c r="F5" s="179"/>
       <c r="H5" s="11"/>
       <c r="I5" s="15" t="s">
         <v>17</v>
@@ -4049,10 +4052,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="205"/>
-      <c r="D6" s="205"/>
-      <c r="E6" s="205"/>
-      <c r="F6" s="205"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
+      <c r="F6" s="179"/>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
@@ -4069,80 +4072,80 @@
       <c r="H7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="204"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="213"/>
-      <c r="L7" s="213"/>
+      <c r="I7" s="180"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="181"/>
     </row>
     <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="204"/>
-      <c r="D8" s="204"/>
-      <c r="E8" s="204"/>
-      <c r="F8" s="204"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="180"/>
+      <c r="F8" s="180"/>
       <c r="H8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="205"/>
-      <c r="J8" s="206"/>
-      <c r="K8" s="206"/>
-      <c r="L8" s="206"/>
+      <c r="I8" s="179"/>
+      <c r="J8" s="185"/>
+      <c r="K8" s="185"/>
+      <c r="L8" s="185"/>
     </row>
     <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="205"/>
-      <c r="F9" s="205"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
       <c r="H9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="205"/>
-      <c r="J9" s="206"/>
-      <c r="K9" s="206"/>
-      <c r="L9" s="206"/>
+      <c r="I9" s="179"/>
+      <c r="J9" s="185"/>
+      <c r="K9" s="185"/>
+      <c r="L9" s="185"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="205"/>
-      <c r="D10" s="205"/>
-      <c r="E10" s="205"/>
-      <c r="F10" s="205"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="179"/>
+      <c r="F10" s="179"/>
       <c r="H10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="205"/>
-      <c r="J10" s="206"/>
-      <c r="K10" s="206"/>
-      <c r="L10" s="206"/>
+      <c r="I10" s="179"/>
+      <c r="J10" s="185"/>
+      <c r="K10" s="185"/>
+      <c r="L10" s="185"/>
     </row>
     <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="205"/>
-      <c r="J11" s="206"/>
-      <c r="K11" s="206"/>
-      <c r="L11" s="206"/>
+      <c r="I11" s="179"/>
+      <c r="J11" s="185"/>
+      <c r="K11" s="185"/>
+      <c r="L11" s="185"/>
     </row>
     <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="18"/>
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="205"/>
-      <c r="J12" s="206"/>
-      <c r="K12" s="206"/>
-      <c r="L12" s="206"/>
+      <c r="I12" s="179"/>
+      <c r="J12" s="185"/>
+      <c r="K12" s="185"/>
+      <c r="L12" s="185"/>
     </row>
     <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="4"/>
@@ -4190,12 +4193,12 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="224"/>
-      <c r="B16" s="225" t="s">
+      <c r="A16" s="231"/>
+      <c r="B16" s="232" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="226"/>
-      <c r="D16" s="226"/>
+      <c r="C16" s="225"/>
+      <c r="D16" s="225"/>
       <c r="E16" s="23"/>
       <c r="F16" s="170"/>
       <c r="G16" s="170"/>
@@ -4209,12 +4212,12 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="224"/>
-      <c r="B17" s="227" t="s">
+      <c r="A17" s="231"/>
+      <c r="B17" s="224" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="226"/>
-      <c r="D17" s="226"/>
+      <c r="C17" s="225"/>
+      <c r="D17" s="225"/>
       <c r="E17" s="23"/>
       <c r="F17" s="170"/>
       <c r="G17" s="170"/>
@@ -4228,11 +4231,11 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="227" t="s">
+      <c r="B18" s="224" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="226"/>
-      <c r="D18" s="226"/>
+      <c r="C18" s="225"/>
+      <c r="D18" s="225"/>
       <c r="E18" s="23"/>
       <c r="F18" s="170"/>
       <c r="G18" s="170"/>
@@ -4246,11 +4249,11 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="231" t="s">
+      <c r="B19" s="229" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="226"/>
-      <c r="D19" s="226"/>
+      <c r="C19" s="225"/>
+      <c r="D19" s="225"/>
       <c r="E19" s="23"/>
       <c r="F19" s="170"/>
       <c r="G19" s="170"/>
@@ -4264,12 +4267,12 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="227" t="s">
+      <c r="B20" s="224" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="226"/>
-      <c r="D20" s="226"/>
-      <c r="E20" s="232"/>
+      <c r="C20" s="225"/>
+      <c r="D20" s="225"/>
+      <c r="E20" s="230"/>
       <c r="F20" s="170"/>
       <c r="G20" s="170"/>
       <c r="H20" s="170"/>
@@ -4282,11 +4285,11 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="227" t="s">
+      <c r="B21" s="224" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="226"/>
-      <c r="D21" s="226"/>
+      <c r="C21" s="225"/>
+      <c r="D21" s="225"/>
       <c r="E21" s="23"/>
       <c r="F21" s="170"/>
       <c r="G21" s="170"/>
@@ -4300,12 +4303,12 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="228" t="s">
+      <c r="B22" s="226" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="229"/>
-      <c r="D22" s="229"/>
-      <c r="E22" s="230"/>
+      <c r="C22" s="227"/>
+      <c r="D22" s="227"/>
+      <c r="E22" s="228"/>
       <c r="F22" s="170"/>
       <c r="G22" s="170"/>
       <c r="H22" s="170"/>
@@ -4481,13 +4484,6 @@
     <row r="66" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:E20"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="I8:L8"/>
@@ -4500,6 +4496,13 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C9:F9"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4518,7 +4521,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -4575,17 +4578,17 @@
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="L4" s="248"/>
     </row>
     <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="205"/>
-      <c r="D5" s="205"/>
-      <c r="E5" s="205"/>
-      <c r="F5" s="205"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="179"/>
+      <c r="E5" s="179"/>
+      <c r="F5" s="179"/>
       <c r="H5" s="11"/>
       <c r="I5" s="15" t="s">
         <v>17</v>
@@ -4599,10 +4602,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="205"/>
-      <c r="D6" s="205"/>
-      <c r="E6" s="205"/>
-      <c r="F6" s="205"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
+      <c r="F6" s="179"/>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
@@ -4619,80 +4622,80 @@
       <c r="H7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="204"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="213"/>
-      <c r="L7" s="214"/>
+      <c r="I7" s="180"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="182"/>
     </row>
     <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="204"/>
-      <c r="D8" s="204"/>
-      <c r="E8" s="204"/>
-      <c r="F8" s="204"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="180"/>
+      <c r="F8" s="180"/>
       <c r="H8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="205"/>
-      <c r="J8" s="206"/>
-      <c r="K8" s="206"/>
-      <c r="L8" s="207"/>
+      <c r="I8" s="179"/>
+      <c r="J8" s="185"/>
+      <c r="K8" s="185"/>
+      <c r="L8" s="186"/>
     </row>
     <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="205"/>
-      <c r="F9" s="205"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
       <c r="H9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="205"/>
-      <c r="J9" s="206"/>
-      <c r="K9" s="206"/>
-      <c r="L9" s="207"/>
+      <c r="I9" s="179"/>
+      <c r="J9" s="185"/>
+      <c r="K9" s="185"/>
+      <c r="L9" s="186"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="205"/>
-      <c r="D10" s="205"/>
-      <c r="E10" s="205"/>
-      <c r="F10" s="205"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="179"/>
+      <c r="F10" s="179"/>
       <c r="H10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="205"/>
-      <c r="J10" s="206"/>
-      <c r="K10" s="206"/>
-      <c r="L10" s="207"/>
+      <c r="I10" s="179"/>
+      <c r="J10" s="185"/>
+      <c r="K10" s="185"/>
+      <c r="L10" s="186"/>
     </row>
     <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="205"/>
-      <c r="J11" s="206"/>
-      <c r="K11" s="206"/>
-      <c r="L11" s="207"/>
+      <c r="I11" s="179"/>
+      <c r="J11" s="185"/>
+      <c r="K11" s="185"/>
+      <c r="L11" s="186"/>
     </row>
     <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="18"/>
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="205"/>
-      <c r="J12" s="206"/>
-      <c r="K12" s="206"/>
-      <c r="L12" s="207"/>
+      <c r="I12" s="179"/>
+      <c r="J12" s="185"/>
+      <c r="K12" s="185"/>
+      <c r="L12" s="186"/>
     </row>
     <row r="13" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
@@ -4733,12 +4736,12 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="224"/>
-      <c r="B15" s="225" t="s">
+      <c r="A15" s="231"/>
+      <c r="B15" s="232" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="226"/>
-      <c r="D15" s="226"/>
+      <c r="C15" s="225"/>
+      <c r="D15" s="225"/>
       <c r="E15" s="23"/>
       <c r="F15" s="170"/>
       <c r="G15" s="170"/>
@@ -4752,12 +4755,12 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="224"/>
-      <c r="B16" s="227" t="s">
+      <c r="A16" s="231"/>
+      <c r="B16" s="224" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="226"/>
-      <c r="D16" s="226"/>
+      <c r="C16" s="225"/>
+      <c r="D16" s="225"/>
       <c r="E16" s="23"/>
       <c r="F16" s="170"/>
       <c r="G16" s="170"/>
@@ -4771,11 +4774,11 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="227" t="s">
+      <c r="B17" s="224" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="226"/>
-      <c r="D17" s="226"/>
+      <c r="C17" s="225"/>
+      <c r="D17" s="225"/>
       <c r="E17" s="23"/>
       <c r="F17" s="170"/>
       <c r="G17" s="170"/>
@@ -4789,11 +4792,11 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="231" t="s">
+      <c r="B18" s="229" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="226"/>
-      <c r="D18" s="226"/>
+      <c r="C18" s="225"/>
+      <c r="D18" s="225"/>
       <c r="E18" s="23"/>
       <c r="F18" s="170"/>
       <c r="G18" s="170"/>
@@ -4825,11 +4828,11 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="227" t="s">
+      <c r="B20" s="224" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="226"/>
-      <c r="D20" s="226"/>
+      <c r="C20" s="225"/>
+      <c r="D20" s="225"/>
       <c r="E20" s="23"/>
       <c r="F20" s="170"/>
       <c r="G20" s="170"/>
@@ -4861,7 +4864,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="228" t="s">
+      <c r="B22" s="226" t="s">
         <v>69</v>
       </c>
       <c r="C22" s="235"/>
@@ -5022,13 +5025,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="I7:L7"/>
     <mergeCell ref="C6:F6"/>
@@ -5041,6 +5037,13 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C9:F9"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="7.874015748031496E-2"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5056,7 +5059,7 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -5113,17 +5116,17 @@
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="L4" s="248"/>
     </row>
     <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="205"/>
-      <c r="D5" s="205"/>
-      <c r="E5" s="205"/>
-      <c r="F5" s="205"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="179"/>
+      <c r="E5" s="179"/>
+      <c r="F5" s="179"/>
       <c r="H5" s="11"/>
       <c r="I5" s="15" t="s">
         <v>17</v>
@@ -5137,10 +5140,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="205"/>
-      <c r="D6" s="205"/>
-      <c r="E6" s="205"/>
-      <c r="F6" s="205"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
+      <c r="F6" s="179"/>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
@@ -5157,79 +5160,79 @@
       <c r="H7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="204"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="213"/>
-      <c r="L7" s="214"/>
+      <c r="I7" s="180"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="182"/>
     </row>
     <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="204"/>
-      <c r="D8" s="204"/>
-      <c r="E8" s="204"/>
-      <c r="F8" s="204"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="180"/>
+      <c r="F8" s="180"/>
       <c r="H8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="205"/>
-      <c r="J8" s="206"/>
-      <c r="K8" s="206"/>
-      <c r="L8" s="207"/>
+      <c r="I8" s="179"/>
+      <c r="J8" s="185"/>
+      <c r="K8" s="185"/>
+      <c r="L8" s="186"/>
     </row>
     <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="205"/>
-      <c r="F9" s="205"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
       <c r="H9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="205"/>
-      <c r="J9" s="206"/>
-      <c r="K9" s="206"/>
-      <c r="L9" s="207"/>
+      <c r="I9" s="179"/>
+      <c r="J9" s="185"/>
+      <c r="K9" s="185"/>
+      <c r="L9" s="186"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="205"/>
-      <c r="D10" s="205"/>
-      <c r="E10" s="205"/>
-      <c r="F10" s="205"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="179"/>
+      <c r="F10" s="179"/>
       <c r="H10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="205"/>
-      <c r="J10" s="206"/>
-      <c r="K10" s="206"/>
-      <c r="L10" s="207"/>
+      <c r="I10" s="179"/>
+      <c r="J10" s="185"/>
+      <c r="K10" s="185"/>
+      <c r="L10" s="186"/>
     </row>
     <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="205"/>
-      <c r="J11" s="206"/>
-      <c r="K11" s="206"/>
-      <c r="L11" s="207"/>
+      <c r="I11" s="179"/>
+      <c r="J11" s="185"/>
+      <c r="K11" s="185"/>
+      <c r="L11" s="186"/>
     </row>
     <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="205"/>
-      <c r="J12" s="206"/>
-      <c r="K12" s="206"/>
-      <c r="L12" s="207"/>
+      <c r="I12" s="179"/>
+      <c r="J12" s="185"/>
+      <c r="K12" s="185"/>
+      <c r="L12" s="186"/>
     </row>
     <row r="13" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
@@ -5270,12 +5273,12 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="224"/>
-      <c r="B15" s="225" t="s">
+      <c r="A15" s="231"/>
+      <c r="B15" s="232" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="226"/>
-      <c r="D15" s="226"/>
+      <c r="C15" s="225"/>
+      <c r="D15" s="225"/>
       <c r="E15" s="23"/>
       <c r="F15" s="170"/>
       <c r="G15" s="170"/>
@@ -5289,12 +5292,12 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="224"/>
-      <c r="B16" s="227" t="s">
+      <c r="A16" s="231"/>
+      <c r="B16" s="224" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="226"/>
-      <c r="D16" s="226"/>
+      <c r="C16" s="225"/>
+      <c r="D16" s="225"/>
       <c r="E16" s="23"/>
       <c r="F16" s="170"/>
       <c r="G16" s="170"/>
@@ -5308,11 +5311,11 @@
       </c>
     </row>
     <row r="17" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="227" t="s">
+      <c r="B17" s="224" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="226"/>
-      <c r="D17" s="226"/>
+      <c r="C17" s="225"/>
+      <c r="D17" s="225"/>
       <c r="E17" s="23"/>
       <c r="F17" s="170"/>
       <c r="G17" s="170"/>
@@ -5344,11 +5347,11 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="227" t="s">
+      <c r="B19" s="224" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="226"/>
-      <c r="D19" s="226"/>
+      <c r="C19" s="225"/>
+      <c r="D19" s="225"/>
       <c r="E19" s="25"/>
       <c r="F19" s="170"/>
       <c r="G19" s="170"/>
@@ -5398,12 +5401,12 @@
       </c>
     </row>
     <row r="22" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="228" t="s">
+      <c r="B22" s="226" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="229"/>
-      <c r="D22" s="229"/>
-      <c r="E22" s="230"/>
+      <c r="C22" s="227"/>
+      <c r="D22" s="227"/>
+      <c r="E22" s="228"/>
       <c r="F22" s="170"/>
       <c r="G22" s="170"/>
       <c r="H22" s="170"/>
@@ -5563,11 +5566,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B22:E22"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="C8:F8"/>
@@ -5581,6 +5579,11 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B22:E22"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5596,7 +5599,7 @@
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -5655,17 +5658,17 @@
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="L4" s="248"/>
     </row>
     <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="205"/>
-      <c r="D5" s="205"/>
-      <c r="E5" s="205"/>
-      <c r="F5" s="205"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="179"/>
+      <c r="E5" s="179"/>
+      <c r="F5" s="179"/>
       <c r="H5" s="11"/>
       <c r="I5" s="15" t="s">
         <v>17</v>
@@ -5679,10 +5682,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="205"/>
-      <c r="D6" s="205"/>
-      <c r="E6" s="205"/>
-      <c r="F6" s="205"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
+      <c r="F6" s="179"/>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
@@ -5699,79 +5702,79 @@
       <c r="H7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="204"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="213"/>
-      <c r="L7" s="214"/>
+      <c r="I7" s="180"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="182"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="204"/>
-      <c r="D8" s="204"/>
-      <c r="E8" s="204"/>
-      <c r="F8" s="204"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="180"/>
+      <c r="F8" s="180"/>
       <c r="H8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="205"/>
-      <c r="J8" s="206"/>
-      <c r="K8" s="206"/>
-      <c r="L8" s="207"/>
+      <c r="I8" s="179"/>
+      <c r="J8" s="185"/>
+      <c r="K8" s="185"/>
+      <c r="L8" s="186"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="205"/>
-      <c r="F9" s="205"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
       <c r="H9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="205"/>
-      <c r="J9" s="206"/>
-      <c r="K9" s="206"/>
-      <c r="L9" s="207"/>
+      <c r="I9" s="179"/>
+      <c r="J9" s="185"/>
+      <c r="K9" s="185"/>
+      <c r="L9" s="186"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="205"/>
-      <c r="D10" s="205"/>
-      <c r="E10" s="205"/>
-      <c r="F10" s="205"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="179"/>
+      <c r="F10" s="179"/>
       <c r="H10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="205"/>
-      <c r="J10" s="206"/>
-      <c r="K10" s="206"/>
-      <c r="L10" s="207"/>
+      <c r="I10" s="179"/>
+      <c r="J10" s="185"/>
+      <c r="K10" s="185"/>
+      <c r="L10" s="186"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="205"/>
-      <c r="J11" s="206"/>
-      <c r="K11" s="206"/>
-      <c r="L11" s="207"/>
+      <c r="I11" s="179"/>
+      <c r="J11" s="185"/>
+      <c r="K11" s="185"/>
+      <c r="L11" s="186"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="205"/>
-      <c r="J12" s="206"/>
-      <c r="K12" s="206"/>
-      <c r="L12" s="207"/>
+      <c r="I12" s="179"/>
+      <c r="J12" s="185"/>
+      <c r="K12" s="185"/>
+      <c r="L12" s="186"/>
     </row>
     <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="4"/>
@@ -6134,8 +6137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -6194,17 +6197,17 @@
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="L4" s="248"/>
     </row>
     <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="205"/>
-      <c r="D5" s="205"/>
-      <c r="E5" s="205"/>
-      <c r="F5" s="205"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="179"/>
+      <c r="E5" s="179"/>
+      <c r="F5" s="179"/>
       <c r="H5" s="11"/>
       <c r="I5" s="15" t="s">
         <v>17</v>
@@ -6218,10 +6221,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="205"/>
-      <c r="D6" s="205"/>
-      <c r="E6" s="205"/>
-      <c r="F6" s="205"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
+      <c r="F6" s="179"/>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
@@ -6238,79 +6241,79 @@
       <c r="H7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="204"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="213"/>
-      <c r="L7" s="214"/>
+      <c r="I7" s="180"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="182"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="204"/>
-      <c r="D8" s="204"/>
-      <c r="E8" s="204"/>
-      <c r="F8" s="204"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="180"/>
+      <c r="F8" s="180"/>
       <c r="H8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="205"/>
-      <c r="J8" s="206"/>
-      <c r="K8" s="206"/>
-      <c r="L8" s="207"/>
+      <c r="I8" s="179"/>
+      <c r="J8" s="185"/>
+      <c r="K8" s="185"/>
+      <c r="L8" s="186"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="205"/>
-      <c r="F9" s="205"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
       <c r="H9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="205"/>
-      <c r="J9" s="206"/>
-      <c r="K9" s="206"/>
-      <c r="L9" s="207"/>
+      <c r="I9" s="179"/>
+      <c r="J9" s="185"/>
+      <c r="K9" s="185"/>
+      <c r="L9" s="186"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="205"/>
-      <c r="D10" s="205"/>
-      <c r="E10" s="205"/>
-      <c r="F10" s="205"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="179"/>
+      <c r="F10" s="179"/>
       <c r="H10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="205"/>
-      <c r="J10" s="206"/>
-      <c r="K10" s="206"/>
-      <c r="L10" s="207"/>
+      <c r="I10" s="179"/>
+      <c r="J10" s="185"/>
+      <c r="K10" s="185"/>
+      <c r="L10" s="186"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="205"/>
-      <c r="J11" s="206"/>
-      <c r="K11" s="206"/>
-      <c r="L11" s="207"/>
+      <c r="I11" s="179"/>
+      <c r="J11" s="185"/>
+      <c r="K11" s="185"/>
+      <c r="L11" s="186"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="205"/>
-      <c r="J12" s="206"/>
-      <c r="K12" s="206"/>
-      <c r="L12" s="207"/>
+      <c r="I12" s="179"/>
+      <c r="J12" s="185"/>
+      <c r="K12" s="185"/>
+      <c r="L12" s="186"/>
     </row>
     <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="4"/>
@@ -6685,8 +6688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A14" zoomScale="110" zoomScaleNormal="120" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:I18"/>
+    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScale="110" zoomScaleNormal="120" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -6745,17 +6748,17 @@
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="L4" s="248"/>
     </row>
     <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="205"/>
-      <c r="D5" s="205"/>
-      <c r="E5" s="205"/>
-      <c r="F5" s="205"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="179"/>
+      <c r="E5" s="179"/>
+      <c r="F5" s="179"/>
       <c r="H5" s="11"/>
       <c r="I5" s="15" t="s">
         <v>17</v>
@@ -6769,10 +6772,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="205"/>
-      <c r="D6" s="205"/>
-      <c r="E6" s="205"/>
-      <c r="F6" s="205"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
+      <c r="F6" s="179"/>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
@@ -6789,80 +6792,80 @@
       <c r="H7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="204"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="213"/>
-      <c r="L7" s="214"/>
+      <c r="I7" s="180"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="182"/>
     </row>
     <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="204"/>
-      <c r="D8" s="204"/>
-      <c r="E8" s="204"/>
-      <c r="F8" s="204"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="180"/>
+      <c r="F8" s="180"/>
       <c r="H8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="205"/>
-      <c r="J8" s="206"/>
-      <c r="K8" s="206"/>
-      <c r="L8" s="207"/>
+      <c r="I8" s="179"/>
+      <c r="J8" s="185"/>
+      <c r="K8" s="185"/>
+      <c r="L8" s="186"/>
     </row>
     <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="205"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="205"/>
-      <c r="F9" s="205"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
       <c r="H9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="205"/>
-      <c r="J9" s="206"/>
-      <c r="K9" s="206"/>
-      <c r="L9" s="207"/>
+      <c r="I9" s="179"/>
+      <c r="J9" s="185"/>
+      <c r="K9" s="185"/>
+      <c r="L9" s="186"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="205"/>
-      <c r="D10" s="205"/>
-      <c r="E10" s="205"/>
-      <c r="F10" s="205"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="179"/>
+      <c r="F10" s="179"/>
       <c r="H10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="205"/>
-      <c r="J10" s="206"/>
-      <c r="K10" s="206"/>
-      <c r="L10" s="207"/>
+      <c r="I10" s="179"/>
+      <c r="J10" s="185"/>
+      <c r="K10" s="185"/>
+      <c r="L10" s="186"/>
     </row>
     <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="205"/>
-      <c r="J11" s="206"/>
-      <c r="K11" s="206"/>
-      <c r="L11" s="207"/>
+      <c r="I11" s="179"/>
+      <c r="J11" s="185"/>
+      <c r="K11" s="185"/>
+      <c r="L11" s="186"/>
     </row>
     <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="18"/>
       <c r="H12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="205"/>
-      <c r="J12" s="206"/>
-      <c r="K12" s="206"/>
-      <c r="L12" s="207"/>
+      <c r="I12" s="179"/>
+      <c r="J12" s="185"/>
+      <c r="K12" s="185"/>
+      <c r="L12" s="186"/>
     </row>
     <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="18"/>
@@ -7054,13 +7057,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="I7:L7"/>
@@ -7072,6 +7068,13 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7083,24 +7086,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7166,10 +7151,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7190,18 +7202,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>